<commit_message>
change to total stress and strain formulation instead of incremental form as in the original formulation
</commit_message>
<xml_diff>
--- a/SDLs.xlsx
+++ b/SDLs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\My Paper\Geotexile and Geomembrane\anal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,6 @@
     <externalReference r:id="rId7"/>
   </externalReferences>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>PE</t>
     <phoneticPr fontId="1"/>
@@ -139,6 +138,30 @@
   </si>
   <si>
     <t xml:space="preserve">       a3 =       2.273  (2.136, 2.411)</t>
+  </si>
+  <si>
+    <t>PP</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PE</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0.5PP</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2PP</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3PP</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4PP</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -373,34 +396,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.12411009023196509</c:v>
+                  <c:v>6.6373637182876019E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.19072253974779704</c:v>
+                  <c:v>0.110942752570691</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.2374413363329626</c:v>
+                  <c:v>0.14514604183816554</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.24947698905508078</c:v>
+                  <c:v>0.16768316172564396</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.26282564432133221</c:v>
+                  <c:v>0.18467157087340852</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3220392153852758</c:v>
+                  <c:v>0.20612339864140558</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.30494334157999914</c:v>
+                  <c:v>0.21935091768130638</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.33064525064428962</c:v>
+                  <c:v>0.23277170779629058</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.29546617235273931</c:v>
+                  <c:v>0.23942090554488499</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.32816665702320613</c:v>
+                  <c:v>0.24806845926385976</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -412,34 +435,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.6909538739917969</c:v>
+                  <c:v>1.7681405943526642</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6027555746450712</c:v>
+                  <c:v>1.6948225671202617</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.546856764002601</c:v>
+                  <c:v>1.6438366865755476</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5065378630281099</c:v>
+                  <c:v>1.6062118822100988</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4761673190222979</c:v>
+                  <c:v>1.5774915657347806</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4520598634137434</c:v>
+                  <c:v>1.5538421792488497</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4320845173354098</c:v>
+                  <c:v>1.5341645347988995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4156299198831406</c:v>
+                  <c:v>1.5181631886766809</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.4020191233857742</c:v>
+                  <c:v>1.5047031015655952</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.3905741223861088</c:v>
+                  <c:v>1.4934035357656923</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -528,28 +551,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.28969974695310946</c:v>
+                  <c:v>0.17872746124239833</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.24886395341707321</c:v>
+                  <c:v>0.19878146460548027</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.36833322513576033</c:v>
+                  <c:v>0.23809968777422619</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.3878220877489264</c:v>
+                  <c:v>0.26675376627979375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.42426694752232513</c:v>
+                  <c:v>0.29239247277710401</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4293248471727919</c:v>
+                  <c:v>0.31158299001978484</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.43167352070841503</c:v>
+                  <c:v>0.32653663827628593</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.46231267287616296</c:v>
+                  <c:v>0.34162324274214445</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -561,28 +584,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.7322564764106896</c:v>
+                  <c:v>1.8274032867570487</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6671504107658244</c:v>
+                  <c:v>1.7710974712384502</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6235078267812537</c:v>
+                  <c:v>1.7312149356228954</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5909360061713129</c:v>
+                  <c:v>1.7000345723760852</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5660912330976451</c:v>
+                  <c:v>1.6770279356474203</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5470482432552271</c:v>
+                  <c:v>1.6587034312572033</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5317723436675272</c:v>
+                  <c:v>1.643924492236746</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.518649905691144</c:v>
+                  <c:v>1.630363889996677</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -671,46 +694,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>-4.5444225039413991E-2</c:v>
+                  <c:v>-2.1895644143307781E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.6460783240644582E-2</c:v>
+                  <c:v>2.0875861810211605E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3.6585791878108835E-2</c:v>
+                  <c:v>5.9947879175552519E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15468043846794832</c:v>
+                  <c:v>3.868181143293406E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-5.7444999005097835E-2</c:v>
+                  <c:v>2.2239097334903039E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.18468715528136079</c:v>
+                  <c:v>4.7968860820986864E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.3728361180953165E-2</c:v>
+                  <c:v>5.4072349075828322E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.11387270641319085</c:v>
+                  <c:v>6.1160683414603824E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.20631084567275165</c:v>
+                  <c:v>7.7071487778270484E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.15455865949953521</c:v>
+                  <c:v>8.4666932328850739E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.14384002374294735</c:v>
+                  <c:v>8.9920598809611063E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.13269958398232701</c:v>
+                  <c:v>9.3414713924521081E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.19792027106704868</c:v>
+                  <c:v>0.10147064900064615</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.19978093166421609</c:v>
+                  <c:v>0.10856127497268256</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -722,46 +745,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>1.6356216271168877</c:v>
+                  <c:v>1.7079939429529858</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5440124208187311</c:v>
+                  <c:v>1.6297105002118593</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4846589622644111</c:v>
+                  <c:v>1.57553165468834</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4417039812757488</c:v>
+                  <c:v>1.5351765352315057</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4090597034444348</c:v>
+                  <c:v>1.5041371948276157</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3831153210120573</c:v>
+                  <c:v>1.4787462801832456</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3618524601923803</c:v>
+                  <c:v>1.4579568320904985</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3442472387769562</c:v>
+                  <c:v>1.4405794126443006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.329224375110359</c:v>
+                  <c:v>1.4254494151173009</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.3161821183565607</c:v>
+                  <c:v>1.4123654303941768</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.3049630913246724</c:v>
+                  <c:v>1.4011841410864352</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.2951491902278758</c:v>
+                  <c:v>1.3911659691909273</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.2864551675378204</c:v>
+                  <c:v>1.3824002451454775</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.2788189027392434</c:v>
+                  <c:v>1.3746732860951418</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -850,31 +873,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.17470012257307291</c:v>
+                  <c:v>8.6592508535044424E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.16675116251814767</c:v>
+                  <c:v>0.11469024359167217</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.36570923758713736</c:v>
+                  <c:v>0.18412430033504151</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.26930372211065978</c:v>
+                  <c:v>0.20222768007438241</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.38184494119119372</c:v>
+                  <c:v>0.23497736987435044</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.30719929375597144</c:v>
+                  <c:v>0.24592919269183505</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.39713728303995188</c:v>
+                  <c:v>0.2663918478354112</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.38669470267197881</c:v>
+                  <c:v>0.28079082864777344</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.32681065067050885</c:v>
+                  <c:v>0.28565350355456676</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -886,31 +909,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.7404396115775711</c:v>
+                  <c:v>1.822371107768963</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6531141584289157</c:v>
+                  <c:v>1.7489501691531595</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5974582636996595</c:v>
+                  <c:v>1.6985885257265272</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5583485062903495</c:v>
+                  <c:v>1.662879935338087</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5290331594502045</c:v>
+                  <c:v>1.6347048341100596</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5056348650184768</c:v>
+                  <c:v>1.6120296624895136</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4865801781327825</c:v>
+                  <c:v>1.5933792362975137</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.470995298159429</c:v>
+                  <c:v>1.5782510813713937</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.4584525263146098</c:v>
+                  <c:v>1.5662099365220228</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -999,43 +1022,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>9.3757671567143527E-2</c:v>
+                  <c:v>2.7573394041877152E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18631381826487642</c:v>
+                  <c:v>8.5406183997936494E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.0498312990989607E-2</c:v>
+                  <c:v>6.0804846032563836E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.21799666289562974</c:v>
+                  <c:v>9.5261831682436737E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.10060326813489413</c:v>
+                  <c:v>9.6195307156505733E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.244239737207229</c:v>
+                  <c:v>0.11937262837492017</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.17776778086874845</c:v>
+                  <c:v>0.12716758995037084</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.16478171135271447</c:v>
+                  <c:v>0.13161878151522965</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.22151517740011265</c:v>
+                  <c:v>0.14128718175166993</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.23784262838028775</c:v>
+                  <c:v>0.15075688065182952</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.24948412813386528</c:v>
+                  <c:v>0.15961529964248958</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.20309288651299057</c:v>
+                  <c:v>0.16314692217255353</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.32020941185176305</c:v>
+                  <c:v>0.17550464028814977</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1047,43 +1070,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1.6545991032687406</c:v>
+                  <c:v>1.7283401707884312</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5643844234460931</c:v>
+                  <c:v>1.6526036207278714</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5063561750312602</c:v>
+                  <c:v>1.5992213376412019</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4641809111583908</c:v>
+                  <c:v>1.5597899620580336</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4322228418598042</c:v>
+                  <c:v>1.5293741073997003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.406955906635972</c:v>
+                  <c:v>1.5048205109399746</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3862244629844778</c:v>
+                  <c:v>1.4843883683047383</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3688997705380646</c:v>
+                  <c:v>1.4672712315986158</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3542817906462632</c:v>
+                  <c:v>1.4527407322187205</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.3417561426741769</c:v>
+                  <c:v>1.4401797814660104</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.3310353500514012</c:v>
+                  <c:v>1.429553048565354</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.321816061075151</c:v>
+                  <c:v>1.4202595012808454</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.3139888388488756</c:v>
+                  <c:v>1.4126303328574779</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1172,49 +1195,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-0.10823439834700059</c:v>
+                  <c:v>-4.6465024530442579E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.10323204689932999</c:v>
+                  <c:v>7.9867423158663468E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.11708881272683309</c:v>
+                  <c:v>-2.4042442583712215E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10308103601261505</c:v>
+                  <c:v>3.6643524566578422E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4.5807528370224913E-2</c:v>
+                  <c:v>-4.932973950305476E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.10093867398941214</c:v>
+                  <c:v>1.157166784599452E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.277374684967114E-2</c:v>
+                  <c:v>1.3047951314597864E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.2824374977670653E-2</c:v>
+                  <c:v>1.776493849310689E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.13529290335262856</c:v>
+                  <c:v>3.0583811480424793E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.5872713688878962E-2</c:v>
+                  <c:v>3.4952703646064814E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.0374139966384284E-2</c:v>
+                  <c:v>3.9887835900711176E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.7945747104243225E-2</c:v>
+                  <c:v>4.4665141855916156E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.5162664289624768E-2</c:v>
+                  <c:v>4.7724823408173883E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.15489416172932804</c:v>
+                  <c:v>5.5484856237205275E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.11309495762463438</c:v>
+                  <c:v>5.9307125568848124E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1226,49 +1249,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1.6235399819788612</c:v>
+                  <c:v>1.6948092528357286</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.530953324207476</c:v>
+                  <c:v>1.6151387088293911</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4707244592370008</c:v>
+                  <c:v>1.5602280093024956</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4273635832401048</c:v>
+                  <c:v>1.5196223438644587</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3943094247322672</c:v>
+                  <c:v>1.4879710640969215</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.367903658004811</c:v>
+                  <c:v>1.4621653972917923</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3462471260541777</c:v>
+                  <c:v>1.4409345995742127</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3281775970539018</c:v>
+                  <c:v>1.4229978744515255</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3128555638706789</c:v>
+                  <c:v>1.4077529432683171</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.299624236942982</c:v>
+                  <c:v>1.3943824330424046</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.2879526989524848</c:v>
+                  <c:v>1.3825255493784567</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.2777264128670414</c:v>
+                  <c:v>1.3722742280835523</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.2687561598004613</c:v>
+                  <c:v>1.3631487756058986</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.2607418217171571</c:v>
+                  <c:v>1.3549676039638074</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.2535900285927311</c:v>
+                  <c:v>1.3477051901862307</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1283,11 +1306,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="316095168"/>
-        <c:axId val="318070560"/>
+        <c:axId val="369440256"/>
+        <c:axId val="369429056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="316095168"/>
+        <c:axId val="369440256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1344,12 +1367,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318070560"/>
+        <c:crossAx val="369429056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="318070560"/>
+        <c:axId val="369429056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.2"/>
@@ -1407,7 +1430,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316095168"/>
+        <c:crossAx val="369440256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2059,82 +2082,82 @@
       <sheetData sheetId="0">
         <row r="4">
           <cell r="AI4">
-            <v>0.12411009023196509</v>
+            <v>6.6373637182876019E-2</v>
           </cell>
           <cell r="AP4">
-            <v>1.6909538739917969</v>
+            <v>1.7681405943526642</v>
           </cell>
         </row>
         <row r="5">
           <cell r="AI5">
-            <v>0.19072253974779704</v>
+            <v>0.110942752570691</v>
           </cell>
           <cell r="AP5">
-            <v>1.6027555746450712</v>
+            <v>1.6948225671202617</v>
           </cell>
         </row>
         <row r="6">
           <cell r="AI6">
-            <v>0.2374413363329626</v>
+            <v>0.14514604183816554</v>
           </cell>
           <cell r="AP6">
-            <v>1.546856764002601</v>
+            <v>1.6438366865755476</v>
           </cell>
         </row>
         <row r="7">
           <cell r="AI7">
-            <v>0.24947698905508078</v>
+            <v>0.16768316172564396</v>
           </cell>
           <cell r="AP7">
-            <v>1.5065378630281099</v>
+            <v>1.6062118822100988</v>
           </cell>
         </row>
         <row r="8">
           <cell r="AI8">
-            <v>0.26282564432133221</v>
+            <v>0.18467157087340852</v>
           </cell>
           <cell r="AP8">
-            <v>1.4761673190222979</v>
+            <v>1.5774915657347806</v>
           </cell>
         </row>
         <row r="9">
           <cell r="AI9">
-            <v>0.3220392153852758</v>
+            <v>0.20612339864140558</v>
           </cell>
           <cell r="AP9">
-            <v>1.4520598634137434</v>
+            <v>1.5538421792488497</v>
           </cell>
         </row>
         <row r="10">
           <cell r="AI10">
-            <v>0.30494334157999914</v>
+            <v>0.21935091768130638</v>
           </cell>
           <cell r="AP10">
-            <v>1.4320845173354098</v>
+            <v>1.5341645347988995</v>
           </cell>
         </row>
         <row r="11">
           <cell r="AI11">
-            <v>0.33064525064428962</v>
+            <v>0.23277170779629058</v>
           </cell>
           <cell r="AP11">
-            <v>1.4156299198831406</v>
+            <v>1.5181631886766809</v>
           </cell>
         </row>
         <row r="12">
           <cell r="AI12">
-            <v>0.29546617235273931</v>
+            <v>0.23942090554488499</v>
           </cell>
           <cell r="AP12">
-            <v>1.4020191233857742</v>
+            <v>1.5047031015655952</v>
           </cell>
         </row>
         <row r="13">
           <cell r="AI13">
-            <v>0.32816665702320613</v>
+            <v>0.24806845926385976</v>
           </cell>
           <cell r="AP13">
-            <v>1.3905741223861088</v>
+            <v>1.4934035357656923</v>
           </cell>
         </row>
       </sheetData>
@@ -2153,66 +2176,66 @@
       <sheetData sheetId="0">
         <row r="5">
           <cell r="AI5">
-            <v>0.28969974695310946</v>
+            <v>0.17872746124239833</v>
           </cell>
           <cell r="AP5">
-            <v>1.7322564764106896</v>
+            <v>1.8274032867570487</v>
           </cell>
         </row>
         <row r="6">
           <cell r="AI6">
-            <v>0.24886395341707321</v>
+            <v>0.19878146460548027</v>
           </cell>
           <cell r="AP6">
-            <v>1.6671504107658244</v>
+            <v>1.7710974712384502</v>
           </cell>
         </row>
         <row r="7">
           <cell r="AI7">
-            <v>0.36833322513576033</v>
+            <v>0.23809968777422619</v>
           </cell>
           <cell r="AP7">
-            <v>1.6235078267812537</v>
+            <v>1.7312149356228954</v>
           </cell>
         </row>
         <row r="8">
           <cell r="AI8">
-            <v>0.3878220877489264</v>
+            <v>0.26675376627979375</v>
           </cell>
           <cell r="AP8">
-            <v>1.5909360061713129</v>
+            <v>1.7000345723760852</v>
           </cell>
         </row>
         <row r="9">
           <cell r="AI9">
-            <v>0.42426694752232513</v>
+            <v>0.29239247277710401</v>
           </cell>
           <cell r="AP9">
-            <v>1.5660912330976451</v>
+            <v>1.6770279356474203</v>
           </cell>
         </row>
         <row r="10">
           <cell r="AI10">
-            <v>0.4293248471727919</v>
+            <v>0.31158299001978484</v>
           </cell>
           <cell r="AP10">
-            <v>1.5470482432552271</v>
+            <v>1.6587034312572033</v>
           </cell>
         </row>
         <row r="11">
           <cell r="AI11">
-            <v>0.43167352070841503</v>
+            <v>0.32653663827628593</v>
           </cell>
           <cell r="AP11">
-            <v>1.5317723436675272</v>
+            <v>1.643924492236746</v>
           </cell>
         </row>
         <row r="12">
           <cell r="AI12">
-            <v>0.46231267287616296</v>
+            <v>0.34162324274214445</v>
           </cell>
           <cell r="AP12">
-            <v>1.518649905691144</v>
+            <v>1.630363889996677</v>
           </cell>
         </row>
       </sheetData>
@@ -2231,114 +2254,114 @@
       <sheetData sheetId="0">
         <row r="4">
           <cell r="AI4">
-            <v>-4.5444225039413991E-2</v>
+            <v>-2.1895644143307781E-2</v>
           </cell>
           <cell r="AP4">
-            <v>1.6356216271168877</v>
+            <v>1.7079939429529858</v>
           </cell>
         </row>
         <row r="5">
           <cell r="AI5">
-            <v>9.6460783240644582E-2</v>
+            <v>2.0875861810211605E-2</v>
           </cell>
           <cell r="AP5">
-            <v>1.5440124208187311</v>
+            <v>1.6297105002118593</v>
           </cell>
         </row>
         <row r="6">
           <cell r="AI6">
-            <v>-3.6585791878108835E-2</v>
+            <v>5.9947879175552519E-3</v>
           </cell>
           <cell r="AP6">
-            <v>1.4846589622644111</v>
+            <v>1.57553165468834</v>
           </cell>
         </row>
         <row r="7">
           <cell r="AI7">
-            <v>0.15468043846794832</v>
+            <v>3.868181143293406E-2</v>
           </cell>
           <cell r="AP7">
-            <v>1.4417039812757488</v>
+            <v>1.5351765352315057</v>
           </cell>
         </row>
         <row r="8">
           <cell r="AI8">
-            <v>-5.7444999005097835E-2</v>
+            <v>2.2239097334903039E-2</v>
           </cell>
           <cell r="AP8">
-            <v>1.4090597034444348</v>
+            <v>1.5041371948276157</v>
           </cell>
         </row>
         <row r="9">
           <cell r="AI9">
-            <v>0.18468715528136079</v>
+            <v>4.7968860820986864E-2</v>
           </cell>
           <cell r="AP9">
-            <v>1.3831153210120573</v>
+            <v>1.4787462801832456</v>
           </cell>
         </row>
         <row r="10">
           <cell r="AI10">
-            <v>9.3728361180953165E-2</v>
+            <v>5.4072349075828322E-2</v>
           </cell>
           <cell r="AP10">
-            <v>1.3618524601923803</v>
+            <v>1.4579568320904985</v>
           </cell>
         </row>
         <row r="11">
           <cell r="AI11">
-            <v>0.11387270641319085</v>
+            <v>6.1160683414603824E-2</v>
           </cell>
           <cell r="AP11">
-            <v>1.3442472387769562</v>
+            <v>1.4405794126443006</v>
           </cell>
         </row>
         <row r="12">
           <cell r="AI12">
-            <v>0.20631084567275165</v>
+            <v>7.7071487778270484E-2</v>
           </cell>
           <cell r="AP12">
-            <v>1.329224375110359</v>
+            <v>1.4254494151173009</v>
           </cell>
         </row>
         <row r="13">
           <cell r="AI13">
-            <v>0.15455865949953521</v>
+            <v>8.4666932328850739E-2</v>
           </cell>
           <cell r="AP13">
-            <v>1.3161821183565607</v>
+            <v>1.4123654303941768</v>
           </cell>
         </row>
         <row r="14">
           <cell r="AI14">
-            <v>0.14384002374294735</v>
+            <v>8.9920598809611063E-2</v>
           </cell>
           <cell r="AP14">
-            <v>1.3049630913246724</v>
+            <v>1.4011841410864352</v>
           </cell>
         </row>
         <row r="15">
           <cell r="AI15">
-            <v>0.13269958398232701</v>
+            <v>9.3414713924521081E-2</v>
           </cell>
           <cell r="AP15">
-            <v>1.2951491902278758</v>
+            <v>1.3911659691909273</v>
           </cell>
         </row>
         <row r="16">
           <cell r="AI16">
-            <v>0.19792027106704868</v>
+            <v>0.10147064900064615</v>
           </cell>
           <cell r="AP16">
-            <v>1.2864551675378204</v>
+            <v>1.3824002451454775</v>
           </cell>
         </row>
         <row r="17">
           <cell r="AI17">
-            <v>0.19978093166421609</v>
+            <v>0.10856127497268256</v>
           </cell>
           <cell r="AP17">
-            <v>1.2788189027392434</v>
+            <v>1.3746732860951418</v>
           </cell>
         </row>
       </sheetData>
@@ -2357,74 +2380,74 @@
       <sheetData sheetId="0">
         <row r="4">
           <cell r="AI4">
-            <v>0.17470012257307291</v>
+            <v>8.6592508535044424E-2</v>
           </cell>
           <cell r="AP4">
-            <v>1.7404396115775711</v>
+            <v>1.822371107768963</v>
           </cell>
         </row>
         <row r="5">
           <cell r="AI5">
-            <v>0.16675116251814767</v>
+            <v>0.11469024359167217</v>
           </cell>
           <cell r="AP5">
-            <v>1.6531141584289157</v>
+            <v>1.7489501691531595</v>
           </cell>
         </row>
         <row r="6">
           <cell r="AI6">
-            <v>0.36570923758713736</v>
+            <v>0.18412430033504151</v>
           </cell>
           <cell r="AP6">
-            <v>1.5974582636996595</v>
+            <v>1.6985885257265272</v>
           </cell>
         </row>
         <row r="7">
           <cell r="AI7">
-            <v>0.26930372211065978</v>
+            <v>0.20222768007438241</v>
           </cell>
           <cell r="AP7">
-            <v>1.5583485062903495</v>
+            <v>1.662879935338087</v>
           </cell>
         </row>
         <row r="8">
           <cell r="AI8">
-            <v>0.38184494119119372</v>
+            <v>0.23497736987435044</v>
           </cell>
           <cell r="AP8">
-            <v>1.5290331594502045</v>
+            <v>1.6347048341100596</v>
           </cell>
         </row>
         <row r="9">
           <cell r="AI9">
-            <v>0.30719929375597144</v>
+            <v>0.24592919269183505</v>
           </cell>
           <cell r="AP9">
-            <v>1.5056348650184768</v>
+            <v>1.6120296624895136</v>
           </cell>
         </row>
         <row r="10">
           <cell r="AI10">
-            <v>0.39713728303995188</v>
+            <v>0.2663918478354112</v>
           </cell>
           <cell r="AP10">
-            <v>1.4865801781327825</v>
+            <v>1.5933792362975137</v>
           </cell>
         </row>
         <row r="11">
           <cell r="AI11">
-            <v>0.38669470267197881</v>
+            <v>0.28079082864777344</v>
           </cell>
           <cell r="AP11">
-            <v>1.470995298159429</v>
+            <v>1.5782510813713937</v>
           </cell>
         </row>
         <row r="12">
           <cell r="AI12">
-            <v>0.32681065067050885</v>
+            <v>0.28565350355456676</v>
           </cell>
           <cell r="AP12">
-            <v>1.4584525263146098</v>
+            <v>1.5662099365220228</v>
           </cell>
         </row>
       </sheetData>
@@ -2443,106 +2466,106 @@
       <sheetData sheetId="0">
         <row r="4">
           <cell r="AI4">
-            <v>9.3757671567143527E-2</v>
+            <v>2.7573394041877152E-2</v>
           </cell>
           <cell r="AP4">
-            <v>1.6545991032687406</v>
+            <v>1.7283401707884312</v>
           </cell>
         </row>
         <row r="5">
           <cell r="AI5">
-            <v>0.18631381826487642</v>
+            <v>8.5406183997936494E-2</v>
           </cell>
           <cell r="AP5">
-            <v>1.5643844234460931</v>
+            <v>1.6526036207278714</v>
           </cell>
         </row>
         <row r="6">
           <cell r="AI6">
-            <v>-1.0498312990989607E-2</v>
+            <v>6.0804846032563836E-2</v>
           </cell>
           <cell r="AP6">
-            <v>1.5063561750312602</v>
+            <v>1.5992213376412019</v>
           </cell>
         </row>
         <row r="7">
           <cell r="AI7">
-            <v>0.21799666289562974</v>
+            <v>9.5261831682436737E-2</v>
           </cell>
           <cell r="AP7">
-            <v>1.4641809111583908</v>
+            <v>1.5597899620580336</v>
           </cell>
         </row>
         <row r="8">
           <cell r="AI8">
-            <v>0.10060326813489413</v>
+            <v>9.6195307156505733E-2</v>
           </cell>
           <cell r="AP8">
-            <v>1.4322228418598042</v>
+            <v>1.5293741073997003</v>
           </cell>
         </row>
         <row r="9">
           <cell r="AI9">
-            <v>0.244239737207229</v>
+            <v>0.11937262837492017</v>
           </cell>
           <cell r="AP9">
-            <v>1.406955906635972</v>
+            <v>1.5048205109399746</v>
           </cell>
         </row>
         <row r="10">
           <cell r="AI10">
-            <v>0.17776778086874845</v>
+            <v>0.12716758995037084</v>
           </cell>
           <cell r="AP10">
-            <v>1.3862244629844778</v>
+            <v>1.4843883683047383</v>
           </cell>
         </row>
         <row r="11">
           <cell r="AI11">
-            <v>0.16478171135271447</v>
+            <v>0.13161878151522965</v>
           </cell>
           <cell r="AP11">
-            <v>1.3688997705380646</v>
+            <v>1.4672712315986158</v>
           </cell>
         </row>
         <row r="12">
           <cell r="AI12">
-            <v>0.22151517740011265</v>
+            <v>0.14128718175166993</v>
           </cell>
           <cell r="AP12">
-            <v>1.3542817906462632</v>
+            <v>1.4527407322187205</v>
           </cell>
         </row>
         <row r="13">
           <cell r="AI13">
-            <v>0.23784262838028775</v>
+            <v>0.15075688065182952</v>
           </cell>
           <cell r="AP13">
-            <v>1.3417561426741769</v>
+            <v>1.4401797814660104</v>
           </cell>
         </row>
         <row r="14">
           <cell r="AI14">
-            <v>0.24948412813386528</v>
+            <v>0.15961529964248958</v>
           </cell>
           <cell r="AP14">
-            <v>1.3310353500514012</v>
+            <v>1.429553048565354</v>
           </cell>
         </row>
         <row r="15">
           <cell r="AI15">
-            <v>0.20309288651299057</v>
+            <v>0.16314692217255353</v>
           </cell>
           <cell r="AP15">
-            <v>1.321816061075151</v>
+            <v>1.4202595012808454</v>
           </cell>
         </row>
         <row r="16">
           <cell r="AI16">
-            <v>0.32020941185176305</v>
+            <v>0.17550464028814977</v>
           </cell>
           <cell r="AP16">
-            <v>1.3139888388488756</v>
+            <v>1.4126303328574779</v>
           </cell>
         </row>
       </sheetData>
@@ -2561,122 +2584,122 @@
       <sheetData sheetId="0">
         <row r="4">
           <cell r="AI4">
-            <v>-0.10823439834700059</v>
+            <v>-4.6465024530442579E-2</v>
           </cell>
           <cell r="AP4">
-            <v>1.6235399819788612</v>
+            <v>1.6948092528357286</v>
           </cell>
         </row>
         <row r="5">
           <cell r="AI5">
-            <v>0.10323204689932999</v>
+            <v>7.9867423158663468E-3</v>
           </cell>
           <cell r="AP5">
-            <v>1.530953324207476</v>
+            <v>1.6151387088293911</v>
           </cell>
         </row>
         <row r="6">
           <cell r="AI6">
-            <v>-0.11708881272683309</v>
+            <v>-2.4042442583712215E-2</v>
           </cell>
           <cell r="AP6">
-            <v>1.4707244592370008</v>
+            <v>1.5602280093024956</v>
           </cell>
         </row>
         <row r="7">
           <cell r="AI7">
-            <v>0.10308103601261505</v>
+            <v>3.6643524566578422E-3</v>
           </cell>
           <cell r="AP7">
-            <v>1.4273635832401048</v>
+            <v>1.5196223438644587</v>
           </cell>
         </row>
         <row r="8">
           <cell r="AI8">
-            <v>-4.5807528370224913E-2</v>
+            <v>-4.932973950305476E-3</v>
           </cell>
           <cell r="AP8">
-            <v>1.3943094247322672</v>
+            <v>1.4879710640969215</v>
           </cell>
         </row>
         <row r="9">
           <cell r="AI9">
-            <v>0.10093867398941214</v>
+            <v>1.157166784599452E-2</v>
           </cell>
           <cell r="AP9">
-            <v>1.367903658004811</v>
+            <v>1.4621653972917923</v>
           </cell>
         </row>
         <row r="10">
           <cell r="AI10">
-            <v>2.277374684967114E-2</v>
+            <v>1.3047951314597864E-2</v>
           </cell>
           <cell r="AP10">
-            <v>1.3462471260541777</v>
+            <v>1.4409345995742127</v>
           </cell>
         </row>
         <row r="11">
           <cell r="AI11">
-            <v>5.2824374977670653E-2</v>
+            <v>1.776493849310689E-2</v>
           </cell>
           <cell r="AP11">
-            <v>1.3281775970539018</v>
+            <v>1.4229978744515255</v>
           </cell>
         </row>
         <row r="12">
           <cell r="AI12">
-            <v>0.13529290335262856</v>
+            <v>3.0583811480424793E-2</v>
           </cell>
           <cell r="AP12">
-            <v>1.3128555638706789</v>
+            <v>1.4077529432683171</v>
           </cell>
         </row>
         <row r="13">
           <cell r="AI13">
-            <v>7.5872713688878962E-2</v>
+            <v>3.4952703646064814E-2</v>
           </cell>
           <cell r="AP13">
-            <v>1.299624236942982</v>
+            <v>1.3943824330424046</v>
           </cell>
         </row>
         <row r="14">
           <cell r="AI14">
-            <v>9.0374139966384284E-2</v>
+            <v>3.9887835900711176E-2</v>
           </cell>
           <cell r="AP14">
-            <v>1.2879526989524848</v>
+            <v>1.3825255493784567</v>
           </cell>
         </row>
         <row r="15">
           <cell r="AI15">
-            <v>9.7945747104243225E-2</v>
+            <v>4.4665141855916156E-2</v>
           </cell>
           <cell r="AP15">
-            <v>1.2777264128670414</v>
+            <v>1.3722742280835523</v>
           </cell>
         </row>
         <row r="16">
           <cell r="AI16">
-            <v>8.5162664289624768E-2</v>
+            <v>4.7724823408173883E-2</v>
           </cell>
           <cell r="AP16">
-            <v>1.2687561598004613</v>
+            <v>1.3631487756058986</v>
           </cell>
         </row>
         <row r="17">
           <cell r="AI17">
-            <v>0.15489416172932804</v>
+            <v>5.5484856237205275E-2</v>
           </cell>
           <cell r="AP17">
-            <v>1.2607418217171571</v>
+            <v>1.3549676039638074</v>
           </cell>
         </row>
         <row r="18">
           <cell r="AI18">
-            <v>0.11309495762463438</v>
+            <v>5.9307125568848124E-2</v>
           </cell>
           <cell r="AP18">
-            <v>1.2535900285927311</v>
+            <v>1.3477051901862307</v>
           </cell>
         </row>
       </sheetData>
@@ -2948,10 +2971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A17:K34"/>
+  <dimension ref="A17:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3232,7 +3255,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:11">
       <c r="A33" s="1" t="s">
         <v>18</v>
       </c>
@@ -3243,7 +3266,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:11">
       <c r="A34" s="1" t="s">
         <v>19</v>
       </c>
@@ -3252,6 +3275,26 @@
       </c>
       <c r="I34" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use Young's modulus where {e_q}^p changes from - to +
</commit_message>
<xml_diff>
--- a/SDLs.xlsx
+++ b/SDLs.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
   <si>
     <t>PE</t>
     <phoneticPr fontId="1"/>
@@ -76,47 +76,8 @@
     <t>General model:</t>
   </si>
   <si>
-    <t xml:space="preserve">     f(x) = a*x+b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       a =     -0.8427  (-1.415, -0.2705)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       b =       1.816  (1.633, 1.998)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       a =     -0.8994  (-1.287, -0.5114)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       b =       1.939  (1.789, 2.089)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       a =      -1.404  (-1.69, -1.118)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       b =       1.863  (1.785, 1.941)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       a =     -0.7655  (-1.401, -0.1305)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       b =       1.561  (1.432, 1.689)</t>
-  </si>
-  <si>
     <t>PE</t>
     <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">       a =     -0.8015  (-1.324, -0.2786)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       b =       1.475  (1.401, 1.549)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       a =     -0.8389  (-1.109, -0.5694)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       b =       1.372  (1.346, 1.399)</t>
   </si>
   <si>
     <t>average</t>
@@ -129,15 +90,6 @@
   <si>
     <t xml:space="preserve">     b(T) = a1*T^a2+a3</t>
     <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">       a1 =     -0.1076  (-0.1771, -0.03802)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       a2 =       0.305  (0.2326, 0.3775)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       a3 =       2.273  (2.136, 2.411)</t>
   </si>
   <si>
     <t>PP</t>
@@ -161,6 +113,75 @@
   </si>
   <si>
     <t>4PP</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ev/eq</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>(q/p)^4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">     y=f(x) = ax+b</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       a =    -0.05144  (-0.05684, -0.04604)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       b =      0.7013  (0.6547, 0.7479)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       a =    -0.05038  (-0.05499, -0.04577)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       b =       0.591  (0.555, 0.627)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       a =    -0.04257  (-0.04652, -0.03862)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       b =      0.4559  (0.4313, 0.4805)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       a =    -0.04116  (-0.04734, -0.03498)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       b =      0.3291  (0.2986, 0.3595)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       a =    -0.05325  (-0.05986, -0.04665)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       b =      0.2957  (0.2671, 0.3243)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       a =    -0.03847  (-0.04397, -0.03297)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       b =      0.1819  (0.1602, 0.2035)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       a =     -0.1047  (-0.2211, 0.01172)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       b =      0.2917  (0.169, 0.4144)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       c =      0.9625  (0.743, 1.182)</t>
+  </si>
+  <si>
+    <t>q/p_0</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -213,13 +234,18 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -238,6 +264,900 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>a</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$46:$B$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>464</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>696</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>928</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$46:$C$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>-5.144E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5.4989999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4.2569999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.4116E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-5.3249999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-3.8469999999999997E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>b</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$46:$B$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>464</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>696</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>928</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$46:$D$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.70130000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59099999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.45590000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3291</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.29570000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.18190000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="346582368"/>
+        <c:axId val="346582928"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="346582368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="346582928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="346582928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="346582368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>a</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$46:$G$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>464</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>696</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>928</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$46:$H$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>-4.2472666666666659E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4.2472666666666659E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4.2472666666666659E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-4.2472666666666659E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.2472666666666659E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-4.2472666666666659E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>b</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$46:$G$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>464</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>696</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>928</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$46:$I$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.63100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.53810000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.45550000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.33539999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1968</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="527969168"/>
+        <c:axId val="579289568"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="527969168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="579289568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="579289568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="527969168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -349,14 +1269,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:intercept val="1.7000000000000002"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.13421083595087163"/>
-                  <c:y val="5.852893028163144E-2"/>
+                  <c:x val="0.15797382195783757"/>
+                  <c:y val="2.922808175016119E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -391,38 +1310,35 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>[1]Sheet1!$AI$4:$AI$13</c:f>
+              <c:f>[1]Sheet1!$AI$5:$AI$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>6.6373637182876019E-2</c:v>
+                  <c:v>0.110942752570691</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.110942752570691</c:v>
+                  <c:v>0.14514604183816554</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.14514604183816554</c:v>
+                  <c:v>0.16768316172564396</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.16768316172564396</c:v>
+                  <c:v>0.18467157087340852</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.18467157087340852</c:v>
+                  <c:v>0.20612339864140558</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.20612339864140558</c:v>
+                  <c:v>0.21935091768130638</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.21935091768130638</c:v>
+                  <c:v>0.23277170779629058</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.23277170779629058</c:v>
+                  <c:v>0.23942090554488499</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.23942090554488499</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>0.24806845926385976</c:v>
                 </c:pt>
               </c:numCache>
@@ -430,38 +1346,35 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>[1]Sheet1!$AP$4:$AP$13</c:f>
+              <c:f>[1]Sheet1!$AQ$5:$AQ$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.7681405943526642</c:v>
+                  <c:v>1.6948225671202617</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6948225671202617</c:v>
+                  <c:v>1.6438366865755476</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6438366865755476</c:v>
+                  <c:v>1.6062118822100988</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6062118822100988</c:v>
+                  <c:v>1.5774915657347806</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5774915657347806</c:v>
+                  <c:v>1.5538421792488497</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5538421792488497</c:v>
+                  <c:v>1.5341645347988995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5341645347988995</c:v>
+                  <c:v>1.5181631886766809</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5181631886766809</c:v>
+                  <c:v>1.5047031015655952</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.5047031015655952</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>1.4934035357656923</c:v>
                 </c:pt>
               </c:numCache>
@@ -579,7 +1492,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>[2]Sheet1!$AP$5:$AP$12</c:f>
+              <c:f>[2]Sheet1!$AQ$5:$AQ$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -653,8 +1566,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.14074907880678256"/>
-                  <c:y val="8.2878271563305211E-2"/>
+                  <c:x val="0.13374118482613423"/>
+                  <c:y val="8.3265733007452283E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -689,50 +1602,41 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>[3]Sheet1!$AI$4:$AI$17</c:f>
+              <c:f>[3]Sheet1!$AI$7:$AI$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>-2.1895644143307781E-2</c:v>
+                  <c:v>3.868181143293406E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0875861810211605E-2</c:v>
+                  <c:v>2.2239097334903039E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.9947879175552519E-3</c:v>
+                  <c:v>4.7968860820986864E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.868181143293406E-2</c:v>
+                  <c:v>5.4072349075828322E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2239097334903039E-2</c:v>
+                  <c:v>6.1160683414603824E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.7968860820986864E-2</c:v>
+                  <c:v>7.7071487778270484E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.4072349075828322E-2</c:v>
+                  <c:v>8.4666932328850739E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.1160683414603824E-2</c:v>
+                  <c:v>8.9920598809611063E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.7071487778270484E-2</c:v>
+                  <c:v>9.3414713924521081E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.4666932328850739E-2</c:v>
+                  <c:v>0.10147064900064615</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.9920598809611063E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>9.3414713924521081E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.10147064900064615</c:v>
-                </c:pt>
-                <c:pt idx="13">
                   <c:v>0.10856127497268256</c:v>
                 </c:pt>
               </c:numCache>
@@ -740,50 +1644,41 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>[3]Sheet1!$AP$4:$AP$17</c:f>
+              <c:f>[3]Sheet1!$AQ$7:$AQ$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.7079939429529858</c:v>
+                  <c:v>1.5351765352315057</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6297105002118593</c:v>
+                  <c:v>1.5041371948276157</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.57553165468834</c:v>
+                  <c:v>1.4787462801832456</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5351765352315057</c:v>
+                  <c:v>1.4579568320904985</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5041371948276157</c:v>
+                  <c:v>1.4405794126443006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4787462801832456</c:v>
+                  <c:v>1.4254494151173009</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4579568320904985</c:v>
+                  <c:v>1.4123654303941768</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4405794126443006</c:v>
+                  <c:v>1.4011841410864352</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.4254494151173009</c:v>
+                  <c:v>1.3911659691909273</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.4123654303941768</c:v>
+                  <c:v>1.3824002451454775</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.4011841410864352</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.3911659691909273</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.3824002451454775</c:v>
-                </c:pt>
-                <c:pt idx="13">
                   <c:v>1.3746732860951418</c:v>
                 </c:pt>
               </c:numCache>
@@ -832,8 +1727,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.15590491795131881"/>
-                  <c:y val="4.2031759613199715E-2"/>
+                  <c:x val="0.19580485125979016"/>
+                  <c:y val="1.6502226687259151E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -904,7 +1799,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>[4]Sheet1!$AP$4:$AP$12</c:f>
+              <c:f>[4]Sheet1!$AQ$4:$AQ$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -915,7 +1810,7 @@
                   <c:v>1.7489501691531595</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6985885257265272</c:v>
+                  <c:v>1.698588525726527</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.662879935338087</c:v>
@@ -981,8 +1876,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.15736252990863342"/>
-                  <c:y val="4.6740017028895457E-2"/>
+                  <c:x val="0.20387518225561699"/>
+                  <c:y val="5.6816511973129806E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1017,47 +1912,41 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>[5]Sheet1!$AI$4:$AI$16</c:f>
+              <c:f>[5]Sheet1!$AI$6:$AI$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2.7573394041877152E-2</c:v>
+                  <c:v>6.0804846032563836E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.5406183997936494E-2</c:v>
+                  <c:v>9.5261831682436737E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0804846032563836E-2</c:v>
+                  <c:v>9.6195307156505733E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.5261831682436737E-2</c:v>
+                  <c:v>0.11937262837492017</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.6195307156505733E-2</c:v>
+                  <c:v>0.12716758995037084</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.11937262837492017</c:v>
+                  <c:v>0.13161878151522965</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.12716758995037084</c:v>
+                  <c:v>0.14128718175166993</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.13161878151522965</c:v>
+                  <c:v>0.15075688065182952</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.14128718175166993</c:v>
+                  <c:v>0.15961529964248958</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.15075688065182952</c:v>
+                  <c:v>0.16314692217255353</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.15961529964248958</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.16314692217255353</c:v>
-                </c:pt>
-                <c:pt idx="12">
                   <c:v>0.17550464028814977</c:v>
                 </c:pt>
               </c:numCache>
@@ -1065,47 +1954,41 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>[5]Sheet1!$AP$4:$AP$16</c:f>
+              <c:f>[5]Sheet1!$AQ$6:$AQ$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.7283401707884312</c:v>
+                  <c:v>1.5992213376412019</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6526036207278714</c:v>
+                  <c:v>1.5597899620580336</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5992213376412019</c:v>
+                  <c:v>1.5293741073997003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5597899620580336</c:v>
+                  <c:v>1.5048205109399746</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5293741073997003</c:v>
+                  <c:v>1.4843883683047383</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5048205109399746</c:v>
+                  <c:v>1.4672712315986158</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4843883683047383</c:v>
+                  <c:v>1.4527407322187205</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4672712315986158</c:v>
+                  <c:v>1.4401797814660104</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.4527407322187205</c:v>
+                  <c:v>1.429553048565354</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.4401797814660104</c:v>
+                  <c:v>1.4202595012808454</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.429553048565354</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.4202595012808454</c:v>
-                </c:pt>
-                <c:pt idx="12">
                   <c:v>1.4126303328574779</c:v>
                 </c:pt>
               </c:numCache>
@@ -1154,8 +2037,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="2.3203399170085667E-2"/>
-                  <c:y val="5.6131030385197969E-2"/>
+                  <c:x val="1.0116986599523353E-2"/>
+                  <c:y val="3.4240002399124322E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1190,53 +2073,41 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>[6]Sheet1!$AI$4:$AI$18</c:f>
+              <c:f>[6]Sheet1!$AI$8:$AI$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>-4.6465024530442579E-2</c:v>
+                  <c:v>-4.932973950305476E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.9867423158663468E-3</c:v>
+                  <c:v>1.157166784599452E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.4042442583712215E-2</c:v>
+                  <c:v>1.3047951314597864E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.6643524566578422E-3</c:v>
+                  <c:v>1.776493849310689E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4.932973950305476E-3</c:v>
+                  <c:v>3.0583811480424793E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.157166784599452E-2</c:v>
+                  <c:v>3.4952703646064814E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3047951314597864E-2</c:v>
+                  <c:v>3.9887835900711176E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.776493849310689E-2</c:v>
+                  <c:v>4.4665141855916156E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0583811480424793E-2</c:v>
+                  <c:v>4.7724823408173883E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.4952703646064814E-2</c:v>
+                  <c:v>5.5484856237205275E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.9887835900711176E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4.4665141855916156E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.7724823408173883E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5.5484856237205275E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
                   <c:v>5.9307125568848124E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -1244,53 +2115,41 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>[6]Sheet1!$AP$4:$AP$18</c:f>
+              <c:f>[6]Sheet1!$AQ$8:$AQ$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.6948092528357286</c:v>
+                  <c:v>1.4879710640969215</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6151387088293911</c:v>
+                  <c:v>1.4621653972917923</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5602280093024956</c:v>
+                  <c:v>1.4409345995742127</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5196223438644587</c:v>
+                  <c:v>1.4229978744515255</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4879710640969215</c:v>
+                  <c:v>1.4077529432683171</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4621653972917923</c:v>
+                  <c:v>1.3943824330424046</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4409345995742127</c:v>
+                  <c:v>1.3825255493784567</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4229978744515255</c:v>
+                  <c:v>1.3722742280835523</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.4077529432683171</c:v>
+                  <c:v>1.3631487756058986</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.3943824330424046</c:v>
+                  <c:v>1.3549676039638074</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.3825255493784567</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.3722742280835523</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.3631487756058986</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.3549676039638074</c:v>
-                </c:pt>
-                <c:pt idx="14">
                   <c:v>1.3477051901862307</c:v>
                 </c:pt>
               </c:numCache>
@@ -1306,11 +2165,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="369440256"/>
-        <c:axId val="369429056"/>
+        <c:axId val="579075440"/>
+        <c:axId val="579069280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="369440256"/>
+        <c:axId val="579075440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1367,12 +2226,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="369429056"/>
+        <c:crossAx val="579069280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="369429056"/>
+        <c:axId val="579069280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.2"/>
@@ -1430,7 +2289,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="369440256"/>
+        <c:crossAx val="579075440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1474,7 +2333,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1519,6 +2378,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2035,8 +2974,1104 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -2048,11 +4083,11 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>575021</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>153040</xdr:rowOff>
+      <xdr:rowOff>38740</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="8" name="Chart 7"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2063,7 +4098,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2085,6 +4120,9 @@
             <v>6.6373637182876019E-2</v>
           </cell>
           <cell r="AP4">
+            <v>101572.6414392595</v>
+          </cell>
+          <cell r="AQ4">
             <v>1.7681405943526642</v>
           </cell>
         </row>
@@ -2092,7 +4130,13 @@
           <cell r="AI5">
             <v>0.110942752570691</v>
           </cell>
+          <cell r="AK5">
+            <v>8.2508169587925995</v>
+          </cell>
           <cell r="AP5">
+            <v>101572.6414392595</v>
+          </cell>
+          <cell r="AQ5">
             <v>1.6948225671202617</v>
           </cell>
         </row>
@@ -2100,7 +4144,13 @@
           <cell r="AI6">
             <v>0.14514604183816554</v>
           </cell>
+          <cell r="AK6">
+            <v>7.3018797173413237</v>
+          </cell>
           <cell r="AP6">
+            <v>101572.6414392595</v>
+          </cell>
+          <cell r="AQ6">
             <v>1.6438366865755476</v>
           </cell>
         </row>
@@ -2108,7 +4158,13 @@
           <cell r="AI7">
             <v>0.16768316172564396</v>
           </cell>
+          <cell r="AK7">
+            <v>6.6559697174068058</v>
+          </cell>
           <cell r="AP7">
+            <v>101572.6414392595</v>
+          </cell>
+          <cell r="AQ7">
             <v>1.6062118822100988</v>
           </cell>
         </row>
@@ -2116,7 +4172,13 @@
           <cell r="AI8">
             <v>0.18467157087340852</v>
           </cell>
+          <cell r="AK8">
+            <v>6.1925309185171971</v>
+          </cell>
           <cell r="AP8">
+            <v>101572.6414392595</v>
+          </cell>
+          <cell r="AQ8">
             <v>1.5774915657347806</v>
           </cell>
         </row>
@@ -2124,7 +4186,13 @@
           <cell r="AI9">
             <v>0.20612339864140558</v>
           </cell>
+          <cell r="AK9">
+            <v>5.8294505820314475</v>
+          </cell>
           <cell r="AP9">
+            <v>101572.6414392595</v>
+          </cell>
+          <cell r="AQ9">
             <v>1.5538421792488497</v>
           </cell>
         </row>
@@ -2132,7 +4200,13 @@
           <cell r="AI10">
             <v>0.21935091768130638</v>
           </cell>
+          <cell r="AK10">
+            <v>5.539719254825064</v>
+          </cell>
           <cell r="AP10">
+            <v>101572.6414392595</v>
+          </cell>
+          <cell r="AQ10">
             <v>1.5341645347988995</v>
           </cell>
         </row>
@@ -2140,7 +4214,13 @@
           <cell r="AI11">
             <v>0.23277170779629058</v>
           </cell>
+          <cell r="AK11">
+            <v>5.312192777550087</v>
+          </cell>
           <cell r="AP11">
+            <v>101572.6414392595</v>
+          </cell>
+          <cell r="AQ11">
             <v>1.5181631886766809</v>
           </cell>
         </row>
@@ -2148,7 +4228,13 @@
           <cell r="AI12">
             <v>0.23942090554488499</v>
           </cell>
+          <cell r="AK12">
+            <v>5.1262911045153903</v>
+          </cell>
           <cell r="AP12">
+            <v>101572.6414392595</v>
+          </cell>
+          <cell r="AQ12">
             <v>1.5047031015655952</v>
           </cell>
         </row>
@@ -2156,7 +4242,13 @@
           <cell r="AI13">
             <v>0.24806845926385976</v>
           </cell>
+          <cell r="AK13">
+            <v>4.9740334426204216</v>
+          </cell>
           <cell r="AP13">
+            <v>101572.6414392595</v>
+          </cell>
+          <cell r="AQ13">
             <v>1.4934035357656923</v>
           </cell>
         </row>
@@ -2178,7 +4270,13 @@
           <cell r="AI5">
             <v>0.17872746124239833</v>
           </cell>
+          <cell r="AK5">
+            <v>11.151610876649848</v>
+          </cell>
           <cell r="AP5">
+            <v>37174.366906725903</v>
+          </cell>
+          <cell r="AQ5">
             <v>1.8274032867570487</v>
           </cell>
         </row>
@@ -2186,7 +4284,13 @@
           <cell r="AI6">
             <v>0.19878146460548027</v>
           </cell>
+          <cell r="AK6">
+            <v>9.8394279946711976</v>
+          </cell>
           <cell r="AP6">
+            <v>37174.366906725903</v>
+          </cell>
+          <cell r="AQ6">
             <v>1.7710974712384502</v>
           </cell>
         </row>
@@ -2194,7 +4298,13 @@
           <cell r="AI7">
             <v>0.23809968777422619</v>
           </cell>
+          <cell r="AK7">
+            <v>8.9826393000799953</v>
+          </cell>
           <cell r="AP7">
+            <v>37174.366906725903</v>
+          </cell>
+          <cell r="AQ7">
             <v>1.7312149356228954</v>
           </cell>
         </row>
@@ -2202,7 +4312,13 @@
           <cell r="AI8">
             <v>0.26675376627979375</v>
           </cell>
+          <cell r="AK8">
+            <v>8.3527794370607289</v>
+          </cell>
           <cell r="AP8">
+            <v>37174.366906725903</v>
+          </cell>
+          <cell r="AQ8">
             <v>1.7000345723760852</v>
           </cell>
         </row>
@@ -2210,7 +4326,13 @@
           <cell r="AI9">
             <v>0.29239247277710401</v>
           </cell>
+          <cell r="AK9">
+            <v>7.9097214262736575</v>
+          </cell>
           <cell r="AP9">
+            <v>37174.366906725903</v>
+          </cell>
+          <cell r="AQ9">
             <v>1.6770279356474203</v>
           </cell>
         </row>
@@ -2218,7 +4340,13 @@
           <cell r="AI10">
             <v>0.31158299001978484</v>
           </cell>
+          <cell r="AK10">
+            <v>7.5696355831523254</v>
+          </cell>
           <cell r="AP10">
+            <v>37174.366906725903</v>
+          </cell>
+          <cell r="AQ10">
             <v>1.6587034312572033</v>
           </cell>
         </row>
@@ -2226,7 +4354,13 @@
           <cell r="AI11">
             <v>0.32653663827628593</v>
           </cell>
+          <cell r="AK11">
+            <v>7.303439964180833</v>
+          </cell>
           <cell r="AP11">
+            <v>37174.366906725903</v>
+          </cell>
+          <cell r="AQ11">
             <v>1.643924492236746</v>
           </cell>
         </row>
@@ -2234,7 +4368,13 @@
           <cell r="AI12">
             <v>0.34162324274214445</v>
           </cell>
+          <cell r="AK12">
+            <v>7.06542338325524</v>
+          </cell>
           <cell r="AP12">
+            <v>37174.366906725903</v>
+          </cell>
+          <cell r="AQ12">
             <v>1.630363889996677</v>
           </cell>
         </row>
@@ -2257,6 +4397,9 @@
             <v>-2.1895644143307781E-2</v>
           </cell>
           <cell r="AP4">
+            <v>302938.08896634029</v>
+          </cell>
+          <cell r="AQ4">
             <v>1.7079939429529858</v>
           </cell>
         </row>
@@ -2265,6 +4408,9 @@
             <v>2.0875861810211605E-2</v>
           </cell>
           <cell r="AP5">
+            <v>302938.08896634029</v>
+          </cell>
+          <cell r="AQ5">
             <v>1.6297105002118593</v>
           </cell>
         </row>
@@ -2273,6 +4419,9 @@
             <v>5.9947879175552519E-3</v>
           </cell>
           <cell r="AP6">
+            <v>302938.08896634029</v>
+          </cell>
+          <cell r="AQ6">
             <v>1.57553165468834</v>
           </cell>
         </row>
@@ -2280,7 +4429,13 @@
           <cell r="AI7">
             <v>3.868181143293406E-2</v>
           </cell>
+          <cell r="AK7">
+            <v>5.5543506655416293</v>
+          </cell>
           <cell r="AP7">
+            <v>302938.08896634029</v>
+          </cell>
+          <cell r="AQ7">
             <v>1.5351765352315057</v>
           </cell>
         </row>
@@ -2288,7 +4443,13 @@
           <cell r="AI8">
             <v>2.2239097334903039E-2</v>
           </cell>
+          <cell r="AK8">
+            <v>5.1185836264926623</v>
+          </cell>
           <cell r="AP8">
+            <v>302938.08896634029</v>
+          </cell>
+          <cell r="AQ8">
             <v>1.5041371948276157</v>
           </cell>
         </row>
@@ -2296,7 +4457,13 @@
           <cell r="AI9">
             <v>4.7968860820986864E-2</v>
           </cell>
+          <cell r="AK9">
+            <v>4.7816156102478056</v>
+          </cell>
           <cell r="AP9">
+            <v>302938.08896634029</v>
+          </cell>
+          <cell r="AQ9">
             <v>1.4787462801832456</v>
           </cell>
         </row>
@@ -2304,7 +4471,13 @@
           <cell r="AI10">
             <v>5.4072349075828322E-2</v>
           </cell>
+          <cell r="AK10">
+            <v>4.5183374352198342</v>
+          </cell>
           <cell r="AP10">
+            <v>302938.08896634029</v>
+          </cell>
+          <cell r="AQ10">
             <v>1.4579568320904985</v>
           </cell>
         </row>
@@ -2312,7 +4485,13 @@
           <cell r="AI11">
             <v>6.1160683414603824E-2</v>
           </cell>
+          <cell r="AK11">
+            <v>4.3067416055433272</v>
+          </cell>
           <cell r="AP11">
+            <v>302938.08896634029</v>
+          </cell>
+          <cell r="AQ11">
             <v>1.4405794126443006</v>
           </cell>
         </row>
@@ -2320,7 +4499,13 @@
           <cell r="AI12">
             <v>7.7071487778270484E-2</v>
           </cell>
+          <cell r="AK12">
+            <v>4.1286421353061593</v>
+          </cell>
           <cell r="AP12">
+            <v>302938.08896634029</v>
+          </cell>
+          <cell r="AQ12">
             <v>1.4254494151173009</v>
           </cell>
         </row>
@@ -2328,7 +4513,13 @@
           <cell r="AI13">
             <v>8.4666932328850739E-2</v>
           </cell>
+          <cell r="AK13">
+            <v>3.9791317249275808</v>
+          </cell>
           <cell r="AP13">
+            <v>302938.08896634029</v>
+          </cell>
+          <cell r="AQ13">
             <v>1.4123654303941768</v>
           </cell>
         </row>
@@ -2336,7 +4527,13 @@
           <cell r="AI14">
             <v>8.9920598809611063E-2</v>
           </cell>
+          <cell r="AK14">
+            <v>3.8546136316205919</v>
+          </cell>
           <cell r="AP14">
+            <v>302938.08896634029</v>
+          </cell>
+          <cell r="AQ14">
             <v>1.4011841410864352</v>
           </cell>
         </row>
@@ -2344,7 +4541,13 @@
           <cell r="AI15">
             <v>9.3414713924521081E-2</v>
           </cell>
+          <cell r="AK15">
+            <v>3.7455515748213779</v>
+          </cell>
           <cell r="AP15">
+            <v>302938.08896634029</v>
+          </cell>
+          <cell r="AQ15">
             <v>1.3911659691909273</v>
           </cell>
         </row>
@@ -2352,7 +4555,13 @@
           <cell r="AI16">
             <v>0.10147064900064615</v>
           </cell>
+          <cell r="AK16">
+            <v>3.6520373341150312</v>
+          </cell>
           <cell r="AP16">
+            <v>302938.08896634029</v>
+          </cell>
+          <cell r="AQ16">
             <v>1.3824002451454775</v>
           </cell>
         </row>
@@ -2360,7 +4569,13 @@
           <cell r="AI17">
             <v>0.10856127497268256</v>
           </cell>
+          <cell r="AK17">
+            <v>3.5710667871674415</v>
+          </cell>
           <cell r="AP17">
+            <v>302938.08896634029</v>
+          </cell>
+          <cell r="AQ17">
             <v>1.3746732860951418</v>
           </cell>
         </row>
@@ -2382,7 +4597,13 @@
           <cell r="AI4">
             <v>8.6592508535044424E-2</v>
           </cell>
+          <cell r="AK4">
+            <v>11.029283131660142</v>
+          </cell>
           <cell r="AP4">
+            <v>77626.17248935283</v>
+          </cell>
+          <cell r="AQ4">
             <v>1.822371107768963</v>
           </cell>
         </row>
@@ -2390,7 +4611,13 @@
           <cell r="AI5">
             <v>0.11469024359167217</v>
           </cell>
+          <cell r="AK5">
+            <v>9.3564207450334393</v>
+          </cell>
           <cell r="AP5">
+            <v>77626.17248935283</v>
+          </cell>
+          <cell r="AQ5">
             <v>1.7489501691531595</v>
           </cell>
         </row>
@@ -2398,15 +4625,27 @@
           <cell r="AI6">
             <v>0.18412430033504151</v>
           </cell>
+          <cell r="AK6">
+            <v>8.3243962342418119</v>
+          </cell>
           <cell r="AP6">
-            <v>1.6985885257265272</v>
+            <v>77626.17248935283</v>
+          </cell>
+          <cell r="AQ6">
+            <v>1.698588525726527</v>
           </cell>
         </row>
         <row r="7">
           <cell r="AI7">
             <v>0.20222768007438241</v>
           </cell>
+          <cell r="AK7">
+            <v>7.6461633555965847</v>
+          </cell>
           <cell r="AP7">
+            <v>77626.17248935283</v>
+          </cell>
+          <cell r="AQ7">
             <v>1.662879935338087</v>
           </cell>
         </row>
@@ -2414,7 +4653,13 @@
           <cell r="AI8">
             <v>0.23497736987435044</v>
           </cell>
+          <cell r="AK8">
+            <v>7.1409729446232255</v>
+          </cell>
           <cell r="AP8">
+            <v>77626.17248935283</v>
+          </cell>
+          <cell r="AQ8">
             <v>1.6347048341100596</v>
           </cell>
         </row>
@@ -2422,7 +4667,13 @@
           <cell r="AI9">
             <v>0.24592919269183505</v>
           </cell>
+          <cell r="AK9">
+            <v>6.7529279408785516</v>
+          </cell>
           <cell r="AP9">
+            <v>77626.17248935283</v>
+          </cell>
+          <cell r="AQ9">
             <v>1.6120296624895136</v>
           </cell>
         </row>
@@ -2430,7 +4681,13 @@
           <cell r="AI10">
             <v>0.2663918478354112</v>
           </cell>
+          <cell r="AK10">
+            <v>6.445796850129458</v>
+          </cell>
           <cell r="AP10">
+            <v>77626.17248935283</v>
+          </cell>
+          <cell r="AQ10">
             <v>1.5933792362975137</v>
           </cell>
         </row>
@@ -2438,7 +4695,13 @@
           <cell r="AI11">
             <v>0.28079082864777344</v>
           </cell>
+          <cell r="AK11">
+            <v>6.2044656179427848</v>
+          </cell>
           <cell r="AP11">
+            <v>77626.17248935283</v>
+          </cell>
+          <cell r="AQ11">
             <v>1.5782510813713937</v>
           </cell>
         </row>
@@ -2446,7 +4709,13 @@
           <cell r="AI12">
             <v>0.28565350355456676</v>
           </cell>
+          <cell r="AK12">
+            <v>6.0172755513511387</v>
+          </cell>
           <cell r="AP12">
+            <v>77626.17248935283</v>
+          </cell>
+          <cell r="AQ12">
             <v>1.5662099365220228</v>
           </cell>
         </row>
@@ -2469,6 +4738,9 @@
             <v>2.7573394041877152E-2</v>
           </cell>
           <cell r="AP4">
+            <v>124294.21369229902</v>
+          </cell>
+          <cell r="AQ4">
             <v>1.7283401707884312</v>
           </cell>
         </row>
@@ -2477,6 +4749,9 @@
             <v>8.5406183997936494E-2</v>
           </cell>
           <cell r="AP5">
+            <v>124294.21369229902</v>
+          </cell>
+          <cell r="AQ5">
             <v>1.6526036207278714</v>
           </cell>
         </row>
@@ -2484,7 +4759,13 @@
           <cell r="AI6">
             <v>6.0804846032563836E-2</v>
           </cell>
+          <cell r="AK6">
+            <v>6.5408517058917441</v>
+          </cell>
           <cell r="AP6">
+            <v>124294.21369229902</v>
+          </cell>
+          <cell r="AQ6">
             <v>1.5992213376412019</v>
           </cell>
         </row>
@@ -2492,7 +4773,13 @@
           <cell r="AI7">
             <v>9.5261831682436737E-2</v>
           </cell>
+          <cell r="AK7">
+            <v>5.9192200384914937</v>
+          </cell>
           <cell r="AP7">
+            <v>124294.21369229902</v>
+          </cell>
+          <cell r="AQ7">
             <v>1.5597899620580336</v>
           </cell>
         </row>
@@ -2500,7 +4787,13 @@
           <cell r="AI8">
             <v>9.6195307156505733E-2</v>
           </cell>
+          <cell r="AK8">
+            <v>5.4708515804995139</v>
+          </cell>
           <cell r="AP8">
+            <v>124294.21369229902</v>
+          </cell>
+          <cell r="AQ8">
             <v>1.5293741073997003</v>
           </cell>
         </row>
@@ -2508,7 +4801,13 @@
           <cell r="AI9">
             <v>0.11937262837492017</v>
           </cell>
+          <cell r="AK9">
+            <v>5.1278912742215805</v>
+          </cell>
           <cell r="AP9">
+            <v>124294.21369229902</v>
+          </cell>
+          <cell r="AQ9">
             <v>1.5048205109399746</v>
           </cell>
         </row>
@@ -2516,7 +4815,13 @@
           <cell r="AI10">
             <v>0.12716758995037084</v>
           </cell>
+          <cell r="AK10">
+            <v>4.8550104631250237</v>
+          </cell>
           <cell r="AP10">
+            <v>124294.21369229902</v>
+          </cell>
+          <cell r="AQ10">
             <v>1.4843883683047383</v>
           </cell>
         </row>
@@ -2524,7 +4829,13 @@
           <cell r="AI11">
             <v>0.13161878151522965</v>
           </cell>
+          <cell r="AK11">
+            <v>4.6349132508888031</v>
+          </cell>
           <cell r="AP11">
+            <v>124294.21369229902</v>
+          </cell>
+          <cell r="AQ11">
             <v>1.4672712315986158</v>
           </cell>
         </row>
@@ -2532,7 +4843,13 @@
           <cell r="AI12">
             <v>0.14128718175166993</v>
           </cell>
+          <cell r="AK12">
+            <v>4.4540229875032571</v>
+          </cell>
           <cell r="AP12">
+            <v>124294.21369229902</v>
+          </cell>
+          <cell r="AQ12">
             <v>1.4527407322187205</v>
           </cell>
         </row>
@@ -2540,7 +4857,13 @@
           <cell r="AI13">
             <v>0.15075688065182952</v>
           </cell>
+          <cell r="AK13">
+            <v>4.301964660487112</v>
+          </cell>
           <cell r="AP13">
+            <v>124294.21369229902</v>
+          </cell>
+          <cell r="AQ13">
             <v>1.4401797814660104</v>
           </cell>
         </row>
@@ -2548,7 +4871,13 @@
           <cell r="AI14">
             <v>0.15961529964248958</v>
           </cell>
+          <cell r="AK14">
+            <v>4.176390546437788</v>
+          </cell>
           <cell r="AP14">
+            <v>124294.21369229902</v>
+          </cell>
+          <cell r="AQ14">
             <v>1.429553048565354</v>
           </cell>
         </row>
@@ -2556,7 +4885,13 @@
           <cell r="AI15">
             <v>0.16314692217255353</v>
           </cell>
+          <cell r="AK15">
+            <v>4.068841882430303</v>
+          </cell>
           <cell r="AP15">
+            <v>124294.21369229902</v>
+          </cell>
+          <cell r="AQ15">
             <v>1.4202595012808454</v>
           </cell>
         </row>
@@ -2564,7 +4899,13 @@
           <cell r="AI16">
             <v>0.17550464028814977</v>
           </cell>
+          <cell r="AK16">
+            <v>3.9821178597184934</v>
+          </cell>
           <cell r="AP16">
+            <v>124294.21369229902</v>
+          </cell>
+          <cell r="AQ16">
             <v>1.4126303328574779</v>
           </cell>
         </row>
@@ -2587,6 +4928,9 @@
             <v>-4.6465024530442579E-2</v>
           </cell>
           <cell r="AP4">
+            <v>327923.30704855063</v>
+          </cell>
+          <cell r="AQ4">
             <v>1.6948092528357286</v>
           </cell>
         </row>
@@ -2595,6 +4939,9 @@
             <v>7.9867423158663468E-3</v>
           </cell>
           <cell r="AP5">
+            <v>327923.30704855063</v>
+          </cell>
+          <cell r="AQ5">
             <v>1.6151387088293911</v>
           </cell>
         </row>
@@ -2603,6 +4950,9 @@
             <v>-2.4042442583712215E-2</v>
           </cell>
           <cell r="AP6">
+            <v>327923.30704855063</v>
+          </cell>
+          <cell r="AQ6">
             <v>1.5602280093024956</v>
           </cell>
         </row>
@@ -2611,6 +4961,9 @@
             <v>3.6643524566578422E-3</v>
           </cell>
           <cell r="AP7">
+            <v>327923.30704855063</v>
+          </cell>
+          <cell r="AQ7">
             <v>1.5196223438644587</v>
           </cell>
         </row>
@@ -2618,7 +4971,13 @@
           <cell r="AI8">
             <v>-4.932973950305476E-3</v>
           </cell>
+          <cell r="AK8">
+            <v>4.9020523295982743</v>
+          </cell>
           <cell r="AP8">
+            <v>327923.30704855063</v>
+          </cell>
+          <cell r="AQ8">
             <v>1.4879710640969215</v>
           </cell>
         </row>
@@ -2626,7 +4985,13 @@
           <cell r="AI9">
             <v>1.157166784599452E-2</v>
           </cell>
+          <cell r="AK9">
+            <v>4.5707346325188603</v>
+          </cell>
           <cell r="AP9">
+            <v>327923.30704855063</v>
+          </cell>
+          <cell r="AQ9">
             <v>1.4621653972917923</v>
           </cell>
         </row>
@@ -2634,7 +4999,13 @@
           <cell r="AI10">
             <v>1.3047951314597864E-2</v>
           </cell>
+          <cell r="AK10">
+            <v>4.310990629646497</v>
+          </cell>
           <cell r="AP10">
+            <v>327923.30704855063</v>
+          </cell>
+          <cell r="AQ10">
             <v>1.4409345995742127</v>
           </cell>
         </row>
@@ -2642,7 +5013,13 @@
           <cell r="AI11">
             <v>1.776493849310689E-2</v>
           </cell>
+          <cell r="AK11">
+            <v>4.1003129562455118</v>
+          </cell>
           <cell r="AP11">
+            <v>327923.30704855063</v>
+          </cell>
+          <cell r="AQ11">
             <v>1.4229978744515255</v>
           </cell>
         </row>
@@ -2650,7 +5027,13 @@
           <cell r="AI12">
             <v>3.0583811480424793E-2</v>
           </cell>
+          <cell r="AK12">
+            <v>3.9274057902103929</v>
+          </cell>
           <cell r="AP12">
+            <v>327923.30704855063</v>
+          </cell>
+          <cell r="AQ12">
             <v>1.4077529432683171</v>
           </cell>
         </row>
@@ -2658,7 +5041,13 @@
           <cell r="AI13">
             <v>3.4952703646064814E-2</v>
           </cell>
+          <cell r="AK13">
+            <v>3.780311704343732</v>
+          </cell>
           <cell r="AP13">
+            <v>327923.30704855063</v>
+          </cell>
+          <cell r="AQ13">
             <v>1.3943824330424046</v>
           </cell>
         </row>
@@ -2666,7 +5055,13 @@
           <cell r="AI14">
             <v>3.9887835900711176E-2</v>
           </cell>
+          <cell r="AK14">
+            <v>3.6533616335326289</v>
+          </cell>
           <cell r="AP14">
+            <v>327923.30704855063</v>
+          </cell>
+          <cell r="AQ14">
             <v>1.3825255493784567</v>
           </cell>
         </row>
@@ -2674,7 +5069,13 @@
           <cell r="AI15">
             <v>4.4665141855916156E-2</v>
           </cell>
+          <cell r="AK15">
+            <v>3.546203292544488</v>
+          </cell>
           <cell r="AP15">
+            <v>327923.30704855063</v>
+          </cell>
+          <cell r="AQ15">
             <v>1.3722742280835523</v>
           </cell>
         </row>
@@ -2682,7 +5083,13 @@
           <cell r="AI16">
             <v>4.7724823408173883E-2</v>
           </cell>
+          <cell r="AK16">
+            <v>3.4528127862433831</v>
+          </cell>
           <cell r="AP16">
+            <v>327923.30704855063</v>
+          </cell>
+          <cell r="AQ16">
             <v>1.3631487756058986</v>
           </cell>
         </row>
@@ -2690,7 +5097,13 @@
           <cell r="AI17">
             <v>5.5484856237205275E-2</v>
           </cell>
+          <cell r="AK17">
+            <v>3.3706654309529607</v>
+          </cell>
           <cell r="AP17">
+            <v>327923.30704855063</v>
+          </cell>
+          <cell r="AQ17">
             <v>1.3549676039638074</v>
           </cell>
         </row>
@@ -2698,7 +5111,13 @@
           <cell r="AI18">
             <v>5.9307125568848124E-2</v>
           </cell>
+          <cell r="AK18">
+            <v>3.2989793993605172</v>
+          </cell>
           <cell r="AP18">
+            <v>327923.30704855063</v>
+          </cell>
+          <cell r="AQ18">
             <v>1.3477051901862307</v>
           </cell>
         </row>
@@ -2971,10 +5390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A17:K37"/>
+  <dimension ref="A18:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="M54" sqref="M54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2982,324 +5401,837 @@
     <col min="1" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="17" spans="1:11">
-      <c r="B17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>10</v>
+    <row r="18" spans="1:13">
+      <c r="A18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="1">
-        <v>53</v>
-      </c>
-      <c r="C18" s="1">
-        <v>-0.89939999999999998</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1.9390000000000001</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G18" s="1">
-        <v>53</v>
-      </c>
-      <c r="H18" s="1">
-        <v>-0.83</v>
-      </c>
-      <c r="I18" s="1">
-        <v>1.913</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>27</v>
+    <row r="19" spans="1:13">
+      <c r="A19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="1">
-        <f>232/2</f>
-        <v>116</v>
-      </c>
-      <c r="C19" s="1">
-        <v>-0.8427</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1.8160000000000001</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1">
-        <f>232/2</f>
-        <v>116</v>
-      </c>
-      <c r="H19" s="1">
-        <v>-0.83</v>
-      </c>
-      <c r="I19" s="1">
-        <v>1.8120000000000001</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>9</v>
+    <row r="20" spans="1:13">
+      <c r="A20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="1">
-        <v>232</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G20" s="1">
-        <v>232</v>
-      </c>
-      <c r="H20" s="1">
-        <v>-0.83</v>
-      </c>
-      <c r="I20" s="1">
-        <v>1.7110000000000001</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>28</v>
-      </c>
+    <row r="21" spans="1:13">
+      <c r="A21" s="2">
+        <v>0.17872746124239833</v>
+      </c>
+      <c r="B21" s="2">
+        <v>11.151610876649848</v>
+      </c>
+      <c r="C21" s="3">
+        <v>8.6592508535044424E-2</v>
+      </c>
+      <c r="D21" s="3">
+        <v>11.029283131660142</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.110942752570691</v>
+      </c>
+      <c r="F21" s="3">
+        <v>8.2508169587925995</v>
+      </c>
+      <c r="G21" s="3">
+        <v>6.0804846032563836E-2</v>
+      </c>
+      <c r="H21" s="1">
+        <v>6.5408517058917441</v>
+      </c>
+      <c r="I21" s="1">
+        <v>3.868181143293406E-2</v>
+      </c>
+      <c r="J21" s="1">
+        <v>5.5543506655416293</v>
+      </c>
+      <c r="K21" s="1">
+        <v>-4.932973950305476E-3</v>
+      </c>
+      <c r="L21" s="1">
+        <v>4.9020523295982743</v>
+      </c>
+      <c r="M21" s="4"/>
     </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="1">
-        <f>B20*2</f>
-        <v>464</v>
-      </c>
-      <c r="C21" s="1">
-        <v>-0.76549999999999996</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1.5609999999999999</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21" s="1">
-        <f>G20*2</f>
-        <v>464</v>
-      </c>
-      <c r="H21" s="1">
-        <v>-0.83</v>
-      </c>
-      <c r="I21" s="1">
-        <v>1.573</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>29</v>
-      </c>
+    <row r="22" spans="1:13">
+      <c r="A22" s="2">
+        <v>0.19878146460548027</v>
+      </c>
+      <c r="B22" s="2">
+        <v>9.8394279946711976</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.11469024359167217</v>
+      </c>
+      <c r="D22" s="3">
+        <v>9.3564207450334393</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.14514604183816554</v>
+      </c>
+      <c r="F22" s="3">
+        <v>7.3018797173413237</v>
+      </c>
+      <c r="G22" s="3">
+        <v>9.5261831682436737E-2</v>
+      </c>
+      <c r="H22" s="1">
+        <v>5.9192200384914937</v>
+      </c>
+      <c r="I22" s="1">
+        <v>2.2239097334903039E-2</v>
+      </c>
+      <c r="J22" s="1">
+        <v>5.1185836264926623</v>
+      </c>
+      <c r="K22" s="1">
+        <v>1.157166784599452E-2</v>
+      </c>
+      <c r="L22" s="1">
+        <v>4.5707346325188603</v>
+      </c>
+      <c r="M22" s="4"/>
     </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="1">
-        <f>B20*3</f>
-        <v>696</v>
-      </c>
-      <c r="C22" s="1">
-        <v>-0.80149999999999999</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1.4750000000000001</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G22" s="1">
-        <f>G20*3</f>
-        <v>696</v>
-      </c>
-      <c r="H22" s="1">
-        <v>-0.83</v>
-      </c>
-      <c r="I22" s="1">
-        <v>1.478</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>30</v>
-      </c>
+    <row r="23" spans="1:13">
+      <c r="A23" s="2">
+        <v>0.23809968777422619</v>
+      </c>
+      <c r="B23" s="2">
+        <v>8.9826393000799953</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.18412430033504151</v>
+      </c>
+      <c r="D23" s="3">
+        <v>8.3243962342418119</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.16768316172564396</v>
+      </c>
+      <c r="F23" s="3">
+        <v>6.6559697174068058</v>
+      </c>
+      <c r="G23" s="3">
+        <v>9.6195307156505733E-2</v>
+      </c>
+      <c r="H23" s="1">
+        <v>5.4708515804995139</v>
+      </c>
+      <c r="I23" s="1">
+        <v>4.7968860820986864E-2</v>
+      </c>
+      <c r="J23" s="1">
+        <v>4.7816156102478056</v>
+      </c>
+      <c r="K23" s="1">
+        <v>1.3047951314597864E-2</v>
+      </c>
+      <c r="L23" s="1">
+        <v>4.310990629646497</v>
+      </c>
+      <c r="M23" s="4"/>
     </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="1">
-        <f>B20*4</f>
-        <v>928</v>
-      </c>
-      <c r="C23" s="1">
-        <v>-0.83889999999999998</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1.3720000000000001</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G23" s="1">
-        <f>G20*4</f>
-        <v>928</v>
-      </c>
-      <c r="H23" s="1">
-        <v>-0.83</v>
-      </c>
-      <c r="I23" s="1">
-        <v>1.411</v>
-      </c>
+    <row r="24" spans="1:13">
+      <c r="A24" s="2">
+        <v>0.26675376627979375</v>
+      </c>
+      <c r="B24" s="2">
+        <v>8.3527794370607289</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.20222768007438241</v>
+      </c>
+      <c r="D24" s="3">
+        <v>7.6461633555965847</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0.18467157087340852</v>
+      </c>
+      <c r="F24" s="3">
+        <v>6.1925309185171971</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0.11937262837492017</v>
+      </c>
+      <c r="H24" s="1">
+        <v>5.1278912742215805</v>
+      </c>
+      <c r="I24" s="1">
+        <v>5.4072349075828322E-2</v>
+      </c>
+      <c r="J24" s="1">
+        <v>4.5183374352198342</v>
+      </c>
+      <c r="K24" s="1">
+        <v>1.776493849310689E-2</v>
+      </c>
+      <c r="L24" s="1">
+        <v>4.1003129562455118</v>
+      </c>
+      <c r="M24" s="4"/>
     </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="1">
-        <f>AVERAGE(C18:C23)</f>
-        <v>-0.82959999999999989</v>
-      </c>
+    <row r="25" spans="1:13">
+      <c r="A25" s="2">
+        <v>0.29239247277710401</v>
+      </c>
+      <c r="B25" s="2">
+        <v>7.9097214262736575</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.23497736987435044</v>
+      </c>
+      <c r="D25" s="1">
+        <v>7.1409729446232255</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0.20612339864140558</v>
+      </c>
+      <c r="F25" s="3">
+        <v>5.8294505820314475</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0.12716758995037084</v>
+      </c>
+      <c r="H25" s="1">
+        <v>4.8550104631250237</v>
+      </c>
+      <c r="I25" s="1">
+        <v>6.1160683414603824E-2</v>
+      </c>
+      <c r="J25" s="1">
+        <v>4.3067416055433272</v>
+      </c>
+      <c r="K25" s="1">
+        <v>3.0583811480424793E-2</v>
+      </c>
+      <c r="L25" s="1">
+        <v>3.9274057902103929</v>
+      </c>
+      <c r="M25" s="4"/>
     </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>10</v>
-      </c>
+    <row r="26" spans="1:13">
+      <c r="A26" s="2">
+        <v>0.31158299001978484</v>
+      </c>
+      <c r="B26" s="2">
+        <v>7.5696355831523254</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.24592919269183505</v>
+      </c>
+      <c r="D26" s="1">
+        <v>6.7529279408785516</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0.21935091768130638</v>
+      </c>
+      <c r="F26" s="3">
+        <v>5.539719254825064</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0.13161878151522965</v>
+      </c>
+      <c r="H26" s="1">
+        <v>4.6349132508888031</v>
+      </c>
+      <c r="I26" s="1">
+        <v>7.7071487778270484E-2</v>
+      </c>
+      <c r="J26" s="1">
+        <v>4.1286421353061593</v>
+      </c>
+      <c r="K26" s="1">
+        <v>3.4952703646064814E-2</v>
+      </c>
+      <c r="L26" s="1">
+        <v>3.780311704343732</v>
+      </c>
+      <c r="M26" s="4"/>
     </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>11</v>
-      </c>
+    <row r="27" spans="1:13">
+      <c r="A27" s="2">
+        <v>0.32653663827628593</v>
+      </c>
+      <c r="B27" s="2">
+        <v>7.303439964180833</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.2663918478354112</v>
+      </c>
+      <c r="D27" s="1">
+        <v>6.445796850129458</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0.23277170779629058</v>
+      </c>
+      <c r="F27" s="3">
+        <v>5.312192777550087</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0.14128718175166993</v>
+      </c>
+      <c r="H27" s="1">
+        <v>4.4540229875032571</v>
+      </c>
+      <c r="I27" s="1">
+        <v>8.4666932328850739E-2</v>
+      </c>
+      <c r="J27" s="1">
+        <v>3.9791317249275808</v>
+      </c>
+      <c r="K27" s="1">
+        <v>3.9887835900711176E-2</v>
+      </c>
+      <c r="L27" s="1">
+        <v>3.6533616335326289</v>
+      </c>
+      <c r="M27" s="4"/>
     </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>9</v>
-      </c>
+    <row r="28" spans="1:13">
+      <c r="A28" s="2">
+        <v>0.34162324274214445</v>
+      </c>
+      <c r="B28" s="2">
+        <v>7.06542338325524</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.28079082864777344</v>
+      </c>
+      <c r="D28" s="1">
+        <v>6.2044656179427848</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0.23942090554488499</v>
+      </c>
+      <c r="F28" s="3">
+        <v>5.1262911045153903</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0.15075688065182952</v>
+      </c>
+      <c r="H28" s="1">
+        <v>4.301964660487112</v>
+      </c>
+      <c r="I28" s="1">
+        <v>8.9920598809611063E-2</v>
+      </c>
+      <c r="J28" s="1">
+        <v>3.8546136316205919</v>
+      </c>
+      <c r="K28" s="1">
+        <v>4.4665141855916156E-2</v>
+      </c>
+      <c r="L28" s="1">
+        <v>3.546203292544488</v>
+      </c>
+      <c r="M28" s="4"/>
     </row>
-    <row r="29" spans="1:11">
-      <c r="A29" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>2</v>
-      </c>
+    <row r="29" spans="1:13">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="1">
+        <v>0.28565350355456676</v>
+      </c>
+      <c r="D29" s="1">
+        <v>6.0172755513511387</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0.24806845926385976</v>
+      </c>
+      <c r="F29" s="3">
+        <v>4.9740334426204216</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0.15961529964248958</v>
+      </c>
+      <c r="H29" s="1">
+        <v>4.176390546437788</v>
+      </c>
+      <c r="I29" s="1">
+        <v>9.3414713924521081E-2</v>
+      </c>
+      <c r="J29" s="1">
+        <v>3.7455515748213779</v>
+      </c>
+      <c r="K29" s="1">
+        <v>4.7724823408173883E-2</v>
+      </c>
+      <c r="L29" s="1">
+        <v>3.4528127862433831</v>
+      </c>
+      <c r="M29" s="4"/>
     </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>16</v>
-      </c>
+    <row r="30" spans="1:13">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3">
+        <v>0.16314692217255353</v>
+      </c>
+      <c r="H30" s="1">
+        <v>4.068841882430303</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0.10147064900064615</v>
+      </c>
+      <c r="J30" s="1">
+        <v>3.6520373341150312</v>
+      </c>
+      <c r="K30" s="1">
+        <v>5.5484856237205275E-2</v>
+      </c>
+      <c r="L30" s="1">
+        <v>3.3706654309529607</v>
+      </c>
+      <c r="M30" s="4"/>
     </row>
-    <row r="31" spans="1:11">
-      <c r="A31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>17</v>
-      </c>
+    <row r="31" spans="1:13">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3">
+        <v>0.17550464028814977</v>
+      </c>
+      <c r="H31" s="1">
+        <v>3.9821178597184934</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0.10856127497268256</v>
+      </c>
+      <c r="J31" s="1">
+        <v>3.5710667871674415</v>
+      </c>
+      <c r="K31" s="1">
+        <v>5.9307125568848124E-2</v>
+      </c>
+      <c r="L31" s="1">
+        <v>3.2989793993605172</v>
+      </c>
+      <c r="M31" s="4"/>
     </row>
-    <row r="32" spans="1:11">
-      <c r="A32" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>5</v>
-      </c>
+    <row r="32" spans="1:13">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="M32" s="4"/>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="E42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I37" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K37" s="1" t="s">
-        <v>36</v>
+      <c r="I43" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="B45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="1">
+        <v>53</v>
+      </c>
+      <c r="C46" s="1">
+        <v>-5.144E-2</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0.70130000000000003</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G46" s="1">
+        <v>53</v>
+      </c>
+      <c r="H46" s="1">
+        <v>-4.2472666666666659E-2</v>
+      </c>
+      <c r="I46" s="1">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="J46" s="1">
+        <f>(-I46/H46)^(1/4)</f>
+        <v>1.9632696707228159</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" s="1">
+        <f>232/2</f>
+        <v>116</v>
+      </c>
+      <c r="C47" s="1">
+        <v>-5.4989999999999997E-2</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G47" s="1">
+        <f>232/2</f>
+        <v>116</v>
+      </c>
+      <c r="H47" s="1">
+        <v>-4.2472666666666659E-2</v>
+      </c>
+      <c r="I47" s="1">
+        <v>0.53810000000000002</v>
+      </c>
+      <c r="J47" s="1">
+        <f t="shared" ref="J47:J51" si="0">(-I47/H47)^(1/4)</f>
+        <v>1.8866370795002798</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" s="1">
+        <v>232</v>
+      </c>
+      <c r="C48" s="1">
+        <v>-4.2569999999999997E-2</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0.45590000000000003</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G48" s="1">
+        <v>232</v>
+      </c>
+      <c r="H48" s="1">
+        <v>-4.2472666666666659E-2</v>
+      </c>
+      <c r="I48" s="1">
+        <v>0.45550000000000002</v>
+      </c>
+      <c r="J48" s="1">
+        <f t="shared" si="0"/>
+        <v>1.8096505244691083</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" s="1">
+        <f>B48*2</f>
+        <v>464</v>
+      </c>
+      <c r="C49" s="1">
+        <v>-1.4116E-2</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0.3291</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G49" s="1">
+        <f>G48*2</f>
+        <v>464</v>
+      </c>
+      <c r="H49" s="1">
+        <v>-4.2472666666666659E-2</v>
+      </c>
+      <c r="I49" s="1">
+        <v>0.33539999999999998</v>
+      </c>
+      <c r="J49" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6763449183153274</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="1">
+        <f>B48*3</f>
+        <v>696</v>
+      </c>
+      <c r="C50" s="1">
+        <v>-5.3249999999999999E-2</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.29570000000000002</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G50" s="1">
+        <f>G48*3</f>
+        <v>696</v>
+      </c>
+      <c r="H50" s="1">
+        <v>-4.2472666666666659E-2</v>
+      </c>
+      <c r="I50" s="1">
+        <v>0.25190000000000001</v>
+      </c>
+      <c r="J50" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5605570843953727</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="1">
+        <f>B48*4</f>
+        <v>928</v>
+      </c>
+      <c r="C51" s="1">
+        <v>-3.8469999999999997E-2</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.18190000000000001</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G51" s="1">
+        <f>G48*4</f>
+        <v>928</v>
+      </c>
+      <c r="H51" s="1">
+        <v>-4.2472666666666659E-2</v>
+      </c>
+      <c r="I51" s="1">
+        <v>0.1968</v>
+      </c>
+      <c r="J51" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4671647739646805</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="1">
+        <f>AVERAGE(C46:C51)</f>
+        <v>-4.2472666666666659E-2</v>
+      </c>
+      <c r="D52" s="1">
+        <f>AVERAGE(D46:D51)</f>
+        <v>0.42581666666666673</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Check validity of equilibrium equations using PE, 0.5PP, PP and 2PP cases
</commit_message>
<xml_diff>
--- a/SDLs.xlsx
+++ b/SDLs.xlsx
@@ -16,8 +16,10 @@
     <sheet name="fit 1" sheetId="2" r:id="rId2"/>
     <sheet name="fit 2" sheetId="3" r:id="rId3"/>
     <sheet name="fit3" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="117">
   <si>
     <t>PE</t>
     <phoneticPr fontId="1"/>
@@ -384,6 +386,53 @@
   <si>
     <t xml:space="preserve">       b =        0.63  (0.622, 0.638)</t>
   </si>
+  <si>
+    <t>b_pred</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>E_pred</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Goodness of fit:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  SSE: 0.001844</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  R-square: 0.9801</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Adjusted R-square: 0.9751</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  RMSE: 0.02147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     b = f(T) = a1*T^a2+0.5483</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       a1 =    0.001449  (0.0003045, 0.002593)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       a2 =      0.7384  (0.6004, 0.8764)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mc^2_pred</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>q/p_pred</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>p_pred</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
@@ -1402,11 +1451,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="333739904"/>
-        <c:axId val="334846800"/>
+        <c:axId val="311164912"/>
+        <c:axId val="311165472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="333739904"/>
+        <c:axId val="311164912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1463,12 +1512,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334846800"/>
+        <c:crossAx val="311165472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="334846800"/>
+        <c:axId val="311165472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.2"/>
@@ -1526,7 +1575,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333739904"/>
+        <c:crossAx val="311164912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2147,11 +2196,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="334852400"/>
-        <c:axId val="334852960"/>
+        <c:axId val="316347360"/>
+        <c:axId val="316347920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="334852400"/>
+        <c:axId val="316347360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2193,12 +2242,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334852960"/>
+        <c:crossAx val="316347920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="334852960"/>
+        <c:axId val="316347920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2249,7 +2298,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334852400"/>
+        <c:crossAx val="316347360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2345,7 +2394,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2767,11 +2815,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="335071360"/>
-        <c:axId val="335071920"/>
+        <c:axId val="314940560"/>
+        <c:axId val="314941120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="335071360"/>
+        <c:axId val="314940560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2828,12 +2876,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335071920"/>
+        <c:crossAx val="314941120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335071920"/>
+        <c:axId val="314941120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2890,7 +2938,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335071360"/>
+        <c:crossAx val="314940560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2904,7 +2952,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2986,7 +3033,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3214,11 +3260,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="335075280"/>
-        <c:axId val="335075840"/>
+        <c:axId val="314944480"/>
+        <c:axId val="314945040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="335075280"/>
+        <c:axId val="314944480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3275,12 +3321,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335075840"/>
+        <c:crossAx val="314945040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335075840"/>
+        <c:axId val="314945040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3337,7 +3383,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335075280"/>
+        <c:crossAx val="314944480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3351,7 +3397,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3433,7 +3478,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3559,8 +3603,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="335126224"/>
-        <c:axId val="335126784"/>
+        <c:axId val="316468560"/>
+        <c:axId val="316469120"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -3757,11 +3801,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="335126224"/>
-        <c:axId val="335126784"/>
+        <c:axId val="316468560"/>
+        <c:axId val="316469120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="335126224"/>
+        <c:axId val="316468560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3818,12 +3862,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335126784"/>
+        <c:crossAx val="316469120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335126784"/>
+        <c:axId val="316469120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3880,7 +3924,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335126224"/>
+        <c:crossAx val="316468560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3894,7 +3938,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4204,11 +4247,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="335130144"/>
-        <c:axId val="335130704"/>
+        <c:axId val="316472480"/>
+        <c:axId val="316473040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="335130144"/>
+        <c:axId val="316472480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4265,12 +4308,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335130704"/>
+        <c:crossAx val="316473040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335130704"/>
+        <c:axId val="316473040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4327,7 +4370,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335130144"/>
+        <c:crossAx val="316472480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4403,7 +4446,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -4651,11 +4694,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="335651520"/>
-        <c:axId val="335652080"/>
+        <c:axId val="481672240"/>
+        <c:axId val="481672800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="335651520"/>
+        <c:axId val="481672240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4712,12 +4755,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335652080"/>
+        <c:crossAx val="481672800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335652080"/>
+        <c:axId val="481672800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4774,7 +4817,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335651520"/>
+        <c:crossAx val="481672240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8945,16 +8988,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>541020</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>138684</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10818,8 +10861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -11214,7 +11257,7 @@
         <v>44381.049882866646</v>
       </c>
       <c r="I26" s="1">
-        <f t="shared" ref="I26:I30" si="4">0.0762*((F26/(1.35*(1-0.0723))*3255000^(-0.0723))^(-1/0.0723))^0.2606-0.5912</f>
+        <f>0.0762*((F26/(1.35*(1-0.0723))*3255000^(-0.0723))^(-1/0.0723))^0.2606-0.5912</f>
         <v>0.23470055794300448</v>
       </c>
     </row>
@@ -11248,7 +11291,7 @@
         <v>70913.089338547434</v>
       </c>
       <c r="I27" s="1">
-        <f t="shared" si="4"/>
+        <f>0.0762*((F27/(1.35*(1-0.0723))*3255000^(-0.0723))^(-1/0.0723))^0.2606-0.5912</f>
         <v>0.38302905119438768</v>
       </c>
     </row>
@@ -11283,7 +11326,7 @@
         <v>144134.92920098061</v>
       </c>
       <c r="I28" s="1">
-        <f t="shared" si="4"/>
+        <f>0.0762*((F28/(1.35*(1-0.0723))*3255000^(-0.0723))^(-1/0.0723))^0.2606-0.5912</f>
         <v>0.65972172512294325</v>
       </c>
     </row>
@@ -11318,7 +11361,7 @@
         <v>295535.22769038728</v>
       </c>
       <c r="I29" s="1">
-        <f t="shared" si="4"/>
+        <f>0.0762*((F29/(1.35*(1-0.0723))*3255000^(-0.0723))^(-1/0.0723))^0.2606-0.5912</f>
         <v>1.0199556691897471</v>
       </c>
     </row>
@@ -11353,7 +11396,7 @@
         <v>650800.06568757712</v>
       </c>
       <c r="I30" s="1">
-        <f t="shared" si="4"/>
+        <f>0.0762*((F30/(1.35*(1-0.0723))*3255000^(-0.0723))^(-1/0.0723))^0.2606-0.5912</f>
         <v>1.5367928505242692</v>
       </c>
     </row>
@@ -11455,16 +11498,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="13.8">
@@ -11755,7 +11799,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" ht="13.8">
+    <row r="17" spans="1:15" ht="13.8">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -11773,7 +11817,7 @@
       </c>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" ht="13.8">
+    <row r="18" spans="1:15" ht="13.8">
       <c r="A18" s="1" t="s">
         <v>87</v>
       </c>
@@ -11791,7 +11835,7 @@
       </c>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" ht="13.8">
+    <row r="19" spans="1:15" ht="13.8">
       <c r="A19" s="1" t="s">
         <v>88</v>
       </c>
@@ -11809,7 +11853,7 @@
       </c>
       <c r="J19" s="1"/>
     </row>
-    <row r="21" spans="1:10" ht="13.8">
+    <row r="21" spans="1:15" ht="13.8">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -11827,7 +11871,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" ht="13.8">
+    <row r="22" spans="1:15" ht="13.8">
       <c r="A22" s="1" t="s">
         <v>95</v>
       </c>
@@ -11845,7 +11889,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" ht="13.8">
+    <row r="23" spans="1:15" ht="13.8">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -11857,7 +11901,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" ht="13.8">
+    <row r="24" spans="1:15" ht="13.8">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>6</v>
@@ -11869,23 +11913,38 @@
         <v>8</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="I24" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="K24" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L24" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="M24" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N24" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="J24" s="1"/>
+      <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="1:10" ht="13.8">
+    <row r="25" spans="1:15" ht="13.8">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -11899,28 +11958,36 @@
         <v>0.5655</v>
       </c>
       <c r="E25" s="1">
-        <f>(9*(1-2*0.33)/(2*D25*(1+0.33))-D25)^2-D25^2</f>
+        <f xml:space="preserve"> 0.001449*B25^0.7384+0.5483</f>
+        <v>0.57548151678369119</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" ref="F25:F30" si="0">(9*(1-2*0.33)/(2*D25*(1+0.33))-D25)^2-D25^2</f>
         <v>1.8374756084274382</v>
       </c>
-      <c r="F25" s="1">
-        <f>D25+SQRT(E25+D25^2)</f>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1">
+        <f t="shared" ref="H25:H30" si="1">D25+SQRT(F25+D25^2)</f>
         <v>2.0342633772760808</v>
       </c>
-      <c r="G25" s="1">
-        <f>(F25/(1.35*(1-0.0723))*3255000^(-0.0723))^(-1/0.0723)</f>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1">
+        <f>(H25/(1.35*(1-0.0723))*3255000^(-0.0723))^(-1/0.0723)</f>
         <v>3969.8770628478278</v>
       </c>
-      <c r="H25" s="1">
-        <f t="shared" ref="H25:H30" si="0">3*(1-2*0.33)/(0.0762*0.2606*G25^(0.2606-1))</f>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1">
+        <f t="shared" ref="L25:L30" si="2">3*(1-2*0.33)/(0.0762*0.2606*J25^(0.2606-1))</f>
         <v>23529.166649066847</v>
       </c>
-      <c r="I25" s="1">
-        <f>-(E25-F25^2)/(2*F25)</f>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1">
+        <f>-(F25-H25^2)/(2*H25)</f>
         <v>0.56550000000000022</v>
       </c>
-      <c r="J25" s="1"/>
+      <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="1:10" ht="13.8">
+    <row r="26" spans="1:15" ht="13.8">
       <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
@@ -11935,28 +12002,36 @@
         <v>0.59919999999999995</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" ref="E26:E30" si="1">(9*(1-2*0.33)/(2*D26*(1+0.33))-D26)^2-D26^2</f>
+        <f t="shared" ref="E26:E30" si="3" xml:space="preserve"> 0.001449*B26^0.7384+0.5483</f>
+        <v>0.59676901173557595</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="0"/>
         <v>1.385083804486547</v>
       </c>
-      <c r="F26" s="1">
-        <f t="shared" ref="F26:F30" si="2">D26+SQRT(E26+D26^2)</f>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1">
+        <f t="shared" si="1"/>
         <v>1.9198530371322162</v>
       </c>
-      <c r="G26" s="1">
-        <f t="shared" ref="G25:G30" si="3">(F26/(1.35*(1-0.0723))*3255000^(-0.0723))^(-1/0.0723)</f>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1">
+        <f t="shared" ref="J26:J30" si="4">(H26/(1.35*(1-0.0723))*3255000^(-0.0723))^(-1/0.0723)</f>
         <v>8840.6413446640327</v>
       </c>
-      <c r="H26" s="1">
-        <f t="shared" si="0"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1">
+        <f t="shared" si="2"/>
         <v>42530.539337002985</v>
       </c>
-      <c r="I26" s="1">
-        <f t="shared" ref="I26:I30" si="4">-(E26-F26^2)/(2*F26)</f>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1">
+        <f>-(F26-H26^2)/(2*H26)</f>
         <v>0.59919999999999995</v>
       </c>
-      <c r="J26" s="1"/>
+      <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="1:10" ht="13.8">
+    <row r="27" spans="1:15" ht="13.8">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -11970,28 +12045,36 @@
         <v>0.63</v>
       </c>
       <c r="E27" s="1">
+        <f t="shared" si="3"/>
+        <v>0.62916204371092588</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0335005843594709</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1">
         <f t="shared" si="1"/>
-        <v>1.0335005843594709</v>
-      </c>
-      <c r="F27" s="1">
+        <v>1.8259935553168631</v>
+      </c>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1">
+        <f t="shared" si="4"/>
+        <v>17683.690742724251</v>
+      </c>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1">
         <f t="shared" si="2"/>
-        <v>1.8259935553168631</v>
-      </c>
-      <c r="G27" s="1">
-        <f t="shared" si="3"/>
-        <v>17683.690742724251</v>
-      </c>
-      <c r="H27" s="1">
-        <f t="shared" si="0"/>
         <v>71011.093371362236</v>
       </c>
-      <c r="I27" s="1">
-        <f t="shared" si="4"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1">
+        <f>-(F27-H27^2)/(2*H27)</f>
         <v>0.63</v>
       </c>
-      <c r="J27" s="1"/>
+      <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="1:10" ht="13.8">
+    <row r="28" spans="1:15" ht="13.8">
       <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
@@ -12006,28 +12089,36 @@
         <v>0.67220000000000002</v>
       </c>
       <c r="E28" s="1">
+        <f t="shared" si="3"/>
+        <v>0.68320413521900503</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="0"/>
+        <v>0.62799988599709133</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1">
         <f t="shared" si="1"/>
-        <v>0.62799988599709133</v>
-      </c>
-      <c r="F28" s="1">
+        <v>1.7113596248878666</v>
+      </c>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1">
+        <f t="shared" si="4"/>
+        <v>43354.374087563447</v>
+      </c>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1">
         <f t="shared" si="2"/>
-        <v>1.7113596248878666</v>
-      </c>
-      <c r="G28" s="1">
-        <f t="shared" si="3"/>
-        <v>43354.374087563447</v>
-      </c>
-      <c r="H28" s="1">
-        <f t="shared" si="0"/>
         <v>137813.87066690897</v>
       </c>
-      <c r="I28" s="1">
-        <f t="shared" si="4"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1">
+        <f>-(F28-H28^2)/(2*H28)</f>
         <v>0.67220000000000024</v>
       </c>
-      <c r="J28" s="1"/>
+      <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="1:10" ht="13.8">
+    <row r="29" spans="1:15" ht="13.8">
       <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
@@ -12042,28 +12133,36 @@
         <v>0.72289999999999999</v>
       </c>
       <c r="E29" s="1">
+        <f t="shared" si="3"/>
+        <v>0.73029147631199187</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="0"/>
+        <v>0.23159462291629251</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1">
         <f t="shared" si="1"/>
-        <v>0.23159462291629251</v>
-      </c>
-      <c r="F29" s="1">
+        <v>1.5913348178857711</v>
+      </c>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1">
+        <f t="shared" si="4"/>
+        <v>118527.77967522097</v>
+      </c>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1">
         <f t="shared" si="2"/>
-        <v>1.5913348178857711</v>
-      </c>
-      <c r="G29" s="1">
-        <f t="shared" si="3"/>
-        <v>118527.77967522097</v>
-      </c>
-      <c r="H29" s="1">
-        <f t="shared" si="0"/>
         <v>289903.46571090003</v>
       </c>
-      <c r="I29" s="1">
-        <f t="shared" si="4"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1">
+        <f>-(F29-H29^2)/(2*H29)</f>
         <v>0.72289999999999988</v>
       </c>
-      <c r="J29" s="1"/>
+      <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="1:10" ht="13.8">
+    <row r="30" spans="1:15" ht="13.8">
       <c r="A30" s="1" t="s">
         <v>5</v>
       </c>
@@ -12078,28 +12177,36 @@
         <v>0.77759999999999996</v>
       </c>
       <c r="E30" s="1">
+        <f t="shared" si="3"/>
+        <v>0.77336388490807551</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.11214844794774154</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1">
         <f t="shared" si="1"/>
-        <v>-0.11214844794774154</v>
-      </c>
-      <c r="F30" s="1">
+        <v>1.4793929267613477</v>
+      </c>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1">
+        <f t="shared" si="4"/>
+        <v>325062.69840798498</v>
+      </c>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1">
         <f t="shared" si="2"/>
-        <v>1.4793929267613477</v>
-      </c>
-      <c r="G30" s="1">
-        <f t="shared" si="3"/>
-        <v>325062.69840798498</v>
-      </c>
-      <c r="H30" s="1">
-        <f t="shared" si="0"/>
         <v>611250.58749924635</v>
       </c>
-      <c r="I30" s="1">
-        <f t="shared" si="4"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1">
+        <f>-(F30-H30^2)/(2*H30)</f>
         <v>0.77759999999999985</v>
       </c>
-      <c r="J30" s="1"/>
+      <c r="O30" s="1"/>
     </row>
-    <row r="31" spans="1:10" ht="13.8">
+    <row r="31" spans="1:15" ht="13.8">
       <c r="A31" s="1" t="s">
         <v>12</v>
       </c>
@@ -12119,7 +12226,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" ht="13.8">
+    <row r="32" spans="1:15" ht="13.8">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -12215,10 +12322,101 @@
       </c>
       <c r="J37" s="1"/>
     </row>
+    <row r="39" spans="1:10" ht="13.8">
+      <c r="G39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" ht="13.8">
+      <c r="G40" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" ht="13.8">
+      <c r="G41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" ht="13.8">
+      <c r="G42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" ht="13.8">
+      <c r="G43" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="1:10" ht="13.8">
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="1:10" ht="13.8">
+      <c r="G45" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="1:10" ht="13.8">
+      <c r="G46" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="1:10" ht="13.8">
+      <c r="G47" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+    </row>
+    <row r="48" spans="1:10" ht="13.8">
+      <c r="G48" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+    </row>
+    <row r="49" spans="7:9" ht="13.8">
+      <c r="G49" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Check equilibrium equations for all cases, sign problem?
</commit_message>
<xml_diff>
--- a/SDLs.xlsx
+++ b/SDLs.xlsx
@@ -19,7 +19,6 @@
     <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1451,11 +1450,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="311164912"/>
-        <c:axId val="311165472"/>
+        <c:axId val="269866160"/>
+        <c:axId val="269866720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="311164912"/>
+        <c:axId val="269866160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1512,12 +1511,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="311165472"/>
+        <c:crossAx val="269866720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="311165472"/>
+        <c:axId val="269866720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.2"/>
@@ -1575,7 +1574,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="311164912"/>
+        <c:crossAx val="269866160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1589,7 +1588,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1671,7 +1669,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2196,11 +2193,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="316347360"/>
-        <c:axId val="316347920"/>
+        <c:axId val="270096080"/>
+        <c:axId val="270096640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="316347360"/>
+        <c:axId val="270096080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2242,12 +2239,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316347920"/>
+        <c:crossAx val="270096640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="316347920"/>
+        <c:axId val="270096640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2298,7 +2295,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316347360"/>
+        <c:crossAx val="270096080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2312,7 +2309,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2815,11 +2811,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="314940560"/>
-        <c:axId val="314941120"/>
+        <c:axId val="270101120"/>
+        <c:axId val="270101680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="314940560"/>
+        <c:axId val="270101120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2876,12 +2872,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314941120"/>
+        <c:crossAx val="270101680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="314941120"/>
+        <c:axId val="270101680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2938,7 +2934,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314940560"/>
+        <c:crossAx val="270101120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3260,11 +3256,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="314944480"/>
-        <c:axId val="314945040"/>
+        <c:axId val="179122960"/>
+        <c:axId val="179123520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="314944480"/>
+        <c:axId val="179122960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3321,12 +3317,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314945040"/>
+        <c:crossAx val="179123520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="314945040"/>
+        <c:axId val="179123520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3383,7 +3379,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314944480"/>
+        <c:crossAx val="179122960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3603,8 +3599,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="316468560"/>
-        <c:axId val="316469120"/>
+        <c:axId val="179127440"/>
+        <c:axId val="179128000"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -3801,11 +3797,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="316468560"/>
-        <c:axId val="316469120"/>
+        <c:axId val="179127440"/>
+        <c:axId val="179128000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="316468560"/>
+        <c:axId val="179127440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3862,12 +3858,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316469120"/>
+        <c:crossAx val="179128000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="316469120"/>
+        <c:axId val="179128000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3924,7 +3920,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316468560"/>
+        <c:crossAx val="179127440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4019,7 +4015,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4247,11 +4242,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="316472480"/>
-        <c:axId val="316473040"/>
+        <c:axId val="270610768"/>
+        <c:axId val="270611328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="316472480"/>
+        <c:axId val="270610768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4308,12 +4303,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316473040"/>
+        <c:crossAx val="270611328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="316473040"/>
+        <c:axId val="270611328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4370,7 +4365,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316472480"/>
+        <c:crossAx val="270610768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4384,7 +4379,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4694,11 +4688,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="481672240"/>
-        <c:axId val="481672800"/>
+        <c:axId val="270614688"/>
+        <c:axId val="270615248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="481672240"/>
+        <c:axId val="270614688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4755,12 +4749,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="481672800"/>
+        <c:crossAx val="270615248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="481672800"/>
+        <c:axId val="270615248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4817,7 +4811,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="481672240"/>
+        <c:crossAx val="270614688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11500,8 +11494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -11962,27 +11956,39 @@
         <v>0.57548151678369119</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" ref="F25:F30" si="0">(9*(1-2*0.33)/(2*D25*(1+0.33))-D25)^2-D25^2</f>
+        <f t="shared" ref="F25:G30" si="0">(9*(1-2*0.33)/(2*D25*(1+0.33))-D25)^2-D25^2</f>
         <v>1.8374756084274382</v>
       </c>
-      <c r="G25" s="1"/>
+      <c r="G25" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6951684481265303</v>
+      </c>
       <c r="H25" s="1">
-        <f t="shared" ref="H25:H30" si="1">D25+SQRT(F25+D25^2)</f>
+        <f t="shared" ref="H25:I30" si="1">D25+SQRT(F25+D25^2)</f>
         <v>2.0342633772760808</v>
       </c>
-      <c r="I25" s="1"/>
+      <c r="I25" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9989798217655372</v>
+      </c>
       <c r="J25" s="1">
         <f>(H25/(1.35*(1-0.0723))*3255000^(-0.0723))^(-1/0.0723)</f>
         <v>3969.8770628478278</v>
       </c>
-      <c r="K25" s="1"/>
+      <c r="K25" s="1">
+        <f>(I25/(1.35*(1-0.0723))*3255000^(-0.0723))^(-1/0.0723)</f>
+        <v>5056.821406939237</v>
+      </c>
       <c r="L25" s="1">
-        <f t="shared" ref="L25:L30" si="2">3*(1-2*0.33)/(0.0762*0.2606*J25^(0.2606-1))</f>
+        <f t="shared" ref="L25:M30" si="2">3*(1-2*0.33)/(0.0762*0.2606*J25^(0.2606-1))</f>
         <v>23529.166649066847</v>
       </c>
-      <c r="M25" s="1"/>
+      <c r="M25" s="1">
+        <f t="shared" si="2"/>
+        <v>28139.598604578088</v>
+      </c>
       <c r="N25" s="1">
-        <f>-(F25-H25^2)/(2*H25)</f>
+        <f t="shared" ref="N25:N30" si="3">-(F25-H25^2)/(2*H25)</f>
         <v>0.56550000000000022</v>
       </c>
       <c r="O25" s="1"/>
@@ -12002,31 +12008,43 @@
         <v>0.59919999999999995</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" ref="E26:E30" si="3" xml:space="preserve"> 0.001449*B26^0.7384+0.5483</f>
+        <f t="shared" ref="E26:E30" si="4" xml:space="preserve"> 0.001449*B26^0.7384+0.5483</f>
         <v>0.59676901173557595</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" si="0"/>
         <v>1.385083804486547</v>
       </c>
-      <c r="G26" s="1"/>
+      <c r="G26" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4151740847261516</v>
+      </c>
       <c r="H26" s="1">
         <f t="shared" si="1"/>
         <v>1.9198530371322162</v>
       </c>
-      <c r="I26" s="1"/>
+      <c r="I26" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9276737183520969</v>
+      </c>
       <c r="J26" s="1">
-        <f t="shared" ref="J26:J30" si="4">(H26/(1.35*(1-0.0723))*3255000^(-0.0723))^(-1/0.0723)</f>
+        <f t="shared" ref="J26:J30" si="5">(H26/(1.35*(1-0.0723))*3255000^(-0.0723))^(-1/0.0723)</f>
         <v>8840.6413446640327</v>
       </c>
-      <c r="K26" s="1"/>
+      <c r="K26" s="1">
+        <f t="shared" ref="K26:K30" si="6">(I26/(1.35*(1-0.0723))*3255000^(-0.0723))^(-1/0.0723)</f>
+        <v>8357.2638951628905</v>
+      </c>
       <c r="L26" s="1">
         <f t="shared" si="2"/>
         <v>42530.539337002985</v>
       </c>
-      <c r="M26" s="1"/>
+      <c r="M26" s="1">
+        <f t="shared" si="2"/>
+        <v>40798.57518375088</v>
+      </c>
       <c r="N26" s="1">
-        <f>-(F26-H26^2)/(2*H26)</f>
+        <f t="shared" si="3"/>
         <v>0.59919999999999995</v>
       </c>
       <c r="O26" s="1"/>
@@ -12045,31 +12063,43 @@
         <v>0.63</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.62916204371092588</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" si="0"/>
         <v>1.0335005843594709</v>
       </c>
-      <c r="G27" s="1"/>
+      <c r="G27" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0423880194203539</v>
+      </c>
       <c r="H27" s="1">
         <f t="shared" si="1"/>
         <v>1.8259935553168631</v>
       </c>
-      <c r="I27" s="1"/>
+      <c r="I27" s="1">
+        <f t="shared" si="1"/>
+        <v>1.8284255246303038</v>
+      </c>
       <c r="J27" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17683.690742724251</v>
       </c>
-      <c r="K27" s="1"/>
+      <c r="K27" s="1">
+        <f t="shared" si="6"/>
+        <v>17361.128840478876</v>
+      </c>
       <c r="L27" s="1">
         <f t="shared" si="2"/>
         <v>71011.093371362236</v>
       </c>
-      <c r="M27" s="1"/>
+      <c r="M27" s="1">
+        <f t="shared" si="2"/>
+        <v>70051.063450813817</v>
+      </c>
       <c r="N27" s="1">
-        <f>-(F27-H27^2)/(2*H27)</f>
+        <f t="shared" si="3"/>
         <v>0.63</v>
       </c>
       <c r="O27" s="1"/>
@@ -12089,31 +12119,43 @@
         <v>0.67220000000000002</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.68320413521900503</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" si="0"/>
         <v>0.62799988599709133</v>
       </c>
-      <c r="G28" s="1"/>
+      <c r="G28" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5344148707525751</v>
+      </c>
       <c r="H28" s="1">
         <f t="shared" si="1"/>
         <v>1.7113596248878666</v>
       </c>
-      <c r="I28" s="1"/>
+      <c r="I28" s="1">
+        <f t="shared" si="1"/>
+        <v>1.6837953410233153</v>
+      </c>
       <c r="J28" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>43354.374087563447</v>
       </c>
-      <c r="K28" s="1"/>
+      <c r="K28" s="1">
+        <f t="shared" si="6"/>
+        <v>54271.353790289635</v>
+      </c>
       <c r="L28" s="1">
         <f t="shared" si="2"/>
         <v>137813.87066690897</v>
       </c>
-      <c r="M28" s="1"/>
+      <c r="M28" s="1">
+        <f t="shared" si="2"/>
+        <v>162709.28305112128</v>
+      </c>
       <c r="N28" s="1">
-        <f>-(F28-H28^2)/(2*H28)</f>
+        <f t="shared" si="3"/>
         <v>0.67220000000000024</v>
       </c>
       <c r="O28" s="1"/>
@@ -12133,31 +12175,43 @@
         <v>0.72289999999999999</v>
       </c>
       <c r="E29" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.73029147631199187</v>
       </c>
       <c r="F29" s="1">
         <f t="shared" si="0"/>
         <v>0.23159462291629251</v>
       </c>
-      <c r="G29" s="1"/>
+      <c r="G29" s="1">
+        <f t="shared" si="0"/>
+        <v>0.18059291755634654</v>
+      </c>
       <c r="H29" s="1">
         <f t="shared" si="1"/>
         <v>1.5913348178857711</v>
       </c>
-      <c r="I29" s="1"/>
+      <c r="I29" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5752284904913301</v>
+      </c>
       <c r="J29" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>118527.77967522097</v>
       </c>
-      <c r="K29" s="1"/>
+      <c r="K29" s="1">
+        <f t="shared" si="6"/>
+        <v>136435.29887168054</v>
+      </c>
       <c r="L29" s="1">
         <f t="shared" si="2"/>
         <v>289903.46571090003</v>
       </c>
-      <c r="M29" s="1"/>
+      <c r="M29" s="1">
+        <f t="shared" si="2"/>
+        <v>321688.56653439248</v>
+      </c>
       <c r="N29" s="1">
-        <f>-(F29-H29^2)/(2*H29)</f>
+        <f t="shared" si="3"/>
         <v>0.72289999999999988</v>
       </c>
       <c r="O29" s="1"/>
@@ -12177,31 +12231,43 @@
         <v>0.77759999999999996</v>
       </c>
       <c r="E30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.77336388490807551</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" si="0"/>
         <v>-0.11214844794774154</v>
       </c>
-      <c r="G30" s="1"/>
+      <c r="G30" s="1">
+        <f t="shared" si="0"/>
+        <v>-8.8106550650407067E-2</v>
+      </c>
       <c r="H30" s="1">
         <f t="shared" si="1"/>
         <v>1.4793929267613477</v>
       </c>
-      <c r="I30" s="1"/>
+      <c r="I30" s="1">
+        <f t="shared" si="1"/>
+        <v>1.4874963290875176</v>
+      </c>
       <c r="J30" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>325062.69840798498</v>
       </c>
-      <c r="K30" s="1"/>
+      <c r="K30" s="1">
+        <f t="shared" si="6"/>
+        <v>301407.7024404651</v>
+      </c>
       <c r="L30" s="1">
         <f t="shared" si="2"/>
         <v>611250.58749924635</v>
       </c>
-      <c r="M30" s="1"/>
+      <c r="M30" s="1">
+        <f t="shared" si="2"/>
+        <v>578039.49484035082</v>
+      </c>
       <c r="N30" s="1">
-        <f>-(F30-H30^2)/(2*H30)</f>
+        <f t="shared" si="3"/>
         <v>0.77759999999999985</v>
       </c>
       <c r="O30" s="1"/>

</xml_diff>

<commit_message>
relate characteristic state line with deviatoric strain, unique relation is found between e_q and q/p-Mf
</commit_message>
<xml_diff>
--- a/SDLs.xlsx
+++ b/SDLs.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="fit 1" sheetId="2" r:id="rId2"/>
-    <sheet name="fit 2" sheetId="3" r:id="rId3"/>
-    <sheet name="fit3" sheetId="4" r:id="rId4"/>
-    <sheet name="fit4" sheetId="5" r:id="rId5"/>
+    <sheet name="e_q-dM" sheetId="6" r:id="rId2"/>
+    <sheet name="fit 1" sheetId="2" r:id="rId3"/>
+    <sheet name="fit 2" sheetId="3" r:id="rId4"/>
+    <sheet name="fit3" sheetId="4" r:id="rId5"/>
+    <sheet name="fit4" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="175">
   <si>
     <t>PE</t>
     <phoneticPr fontId="1"/>
@@ -593,6 +594,35 @@
   </si>
   <si>
     <t>p</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>eq</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>dratio-M</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       a =      -1.386  (-1.422, -1.349)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       b =     0.03463  (0.02994, 0.03933)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       c =        1.27  (1.238, 1.302)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     f(x) = a/(x+c)+b</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> -1.386/(x+1.27)+0.03463</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>f(x)=</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -600,7 +630,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -621,6 +651,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="HGGothicE"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="2">
@@ -645,7 +681,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -657,6 +693,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1574,11 +1615,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="371558592"/>
-        <c:axId val="371559152"/>
+        <c:axId val="426527552"/>
+        <c:axId val="426528112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="371558592"/>
+        <c:axId val="426527552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1635,12 +1676,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371559152"/>
+        <c:crossAx val="426528112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="371559152"/>
+        <c:axId val="426528112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.2"/>
@@ -1698,7 +1739,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371558592"/>
+        <c:crossAx val="426527552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2553,11 +2594,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="371564752"/>
-        <c:axId val="371565312"/>
+        <c:axId val="395532848"/>
+        <c:axId val="395533408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="371564752"/>
+        <c:axId val="395532848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2600,12 +2641,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371565312"/>
+        <c:crossAx val="395533408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="371565312"/>
+        <c:axId val="395533408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2656,7 +2697,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371564752"/>
+        <c:crossAx val="395532848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2752,6 +2793,803 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'e_q-dM'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>dratio-M</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'e_q-dM'!$A$2:$A$460</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="459"/>
+                <c:pt idx="0">
+                  <c:v>1.1782426886005244E-9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83001552430559766</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7589948652665472</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7416603735437604</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.7576796987193877</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.7930546241118881</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.8349244772073154</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.914758087843035</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.9833701226127234</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.0780800075120371</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.15510136159808</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.251465412258712</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.439201033993605</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.8712636408795333E-8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.60385484924843991</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5489256315891522</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.5823189195798366</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.616329679161276</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.708119553395461</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.8224228299217398</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.9544037559349565</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.087888554101534</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.2382312100566431</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10.393042696659142</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>11.595556534490276</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12.760909153627127</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.588996263687477E-10</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.86439544855037098</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.8270880839220307</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.8131835652496848</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.8888826306841788</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.9384663104565565</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6.0396844916037837</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7.1192576157988006</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8.2334755863341869</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.3529214808213137</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>10.457959603650322</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7.7290840394539373E-9</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.78881789650508294</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.6964328109948899</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2.6687025817170649</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.5894703995944859</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.5971902850329718</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5.5707389170981036</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>6.6047566541380522</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>7.6222196992331996</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>8.6452885353400131</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>9.6871456706652967</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>10.740525300466734</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>11.799224683651081</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>12.842394085569522</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>13.939128383436827</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.531280308865322E-6</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.79227428895571161</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.6467493256652945</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.5786011719554747</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.4797714886515165</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.46032940890486</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.3807128307200633</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>6.3933386030602106</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>7.3773424148796956</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>8.3693944476711231</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>9.3997601185372393</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>10.42127381778735</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>11.4366759110223</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>12.453888443639299</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>13.494096944178469</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>14.54301115556521</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>7.9876845878364592E-11</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.78844564873822742</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.6206165472530574</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2.5471234733867654</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3.4239152124484211</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4.3781385242079391</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>5.2990118274572842</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>6.2776536759509556</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7.2305419317242237</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>8.203357726998961</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>9.2076430177192403</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>10.190712166579036</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>11.186873665065443</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>12.189923798057709</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>13.186169417201416</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>14.215500696200856</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>15.2256821864807</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'e_q-dM'!$B$2:$B$460</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="459"/>
+                <c:pt idx="0">
+                  <c:v>-0.99838277802482045</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.61322306275872585</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.41727233784336892</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.32374989669132503</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.24633235668020714</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.19388056967841982</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.15963684492845132</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.13341414332915869</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.11190766491172366</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.10276467581223292</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-9.6729723684952029E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-9.5309040439308212E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.10109273789013917</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.88456311129873444</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.73431037601183302</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.45582422382012289</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.31559189530742793</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-0.23638655876496029</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-0.18286450000625365</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.13944309096909246</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-0.11365219534445625</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-9.6291770225417128E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-8.7196058035180712E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-7.3336627598270976E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-7.2686623801271555E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-7.4157477540880867E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.92434352155457233</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-0.59815475352698999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-0.40110825976505105</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-0.29905086934963232</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-0.22886711701219875</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-0.1807216286625184</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-0.14746945952397716</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-0.12446302052617675</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-0.10663731850704128</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-9.8306426218596199E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-9.9555822995210042E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-1.0562220670498046</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-0.63829438716569076</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-0.44991380847956175</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-0.34624293348388746</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-0.2628987505077478</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-0.20456733607634736</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-0.16376198830805255</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-0.13465652468058642</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-0.11284757798230438</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-0.10143163209276063</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-9.3923477877279726E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-8.8678819210161741E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-8.8437284218419121E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-9.1079591729153364E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-9.7868975529099345E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-1.0847555143299736</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-0.65187030070274132</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-0.4663050017803767</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-0.35793676363642857</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-0.27094612035282473</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-0.20887469804261061</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-0.16786683170051719</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-0.13465370863326354</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-0.11345849214686354</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-0.10010041669404979</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-8.9122978407390807E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-8.379704998582671E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-8.4116996567273006E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-8.3057565743880346E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-8.323701551483409E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-8.6810945894206348E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-1.0995759540501888</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-0.66382382103749893</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-0.47891719273122968</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-0.3654935415169227</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-0.27541389757369683</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-0.21394633105404237</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-0.17055529153211646</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-0.13657785299767022</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-0.11350037110808553</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-9.7663731690701416E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-8.9153432811833966E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-8.2507518707066962E-2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-7.688281361434246E-2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-7.7829370367991313E-2</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-7.8348070535637859E-2</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-8.1000224638744456E-2</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-8.4421040578937179E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="405334448"/>
+        <c:axId val="404926144"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="405334448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="404926144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="404926144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="405334448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3173,11 +4011,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="371569232"/>
-        <c:axId val="371569792"/>
+        <c:axId val="426837024"/>
+        <c:axId val="403565840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="371569232"/>
+        <c:axId val="426837024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3234,12 +4072,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371569792"/>
+        <c:crossAx val="403565840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="371569792"/>
+        <c:axId val="403565840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3296,7 +4134,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371569232"/>
+        <c:crossAx val="426837024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3376,7 +4214,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3391,7 +4229,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3619,11 +4456,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="371573152"/>
-        <c:axId val="371573712"/>
+        <c:axId val="403569200"/>
+        <c:axId val="405447024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="371573152"/>
+        <c:axId val="403569200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3680,12 +4517,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371573712"/>
+        <c:crossAx val="405447024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="371573712"/>
+        <c:axId val="405447024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3742,7 +4579,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371573152"/>
+        <c:crossAx val="403569200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3756,550 +4593,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ja-JP"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="ja-JP"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ja-JP"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'fit 2'!$D$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>b</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'fit 2'!$B$5:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>116</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>232</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>464</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>696</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>928</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'fit 2'!$E$25:$E$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.5433019783579935</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.4918040551445935</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.4014353519810159</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.2367890716512302</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0914861007278438</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.96325390916619147</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="371746032"/>
-        <c:axId val="371746592"/>
-      </c:scatterChart>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'fit 2'!$D$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>b</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'fit 2'!$B$5:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>116</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>232</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>464</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>696</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>928</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'fit 2'!$D$25:$D$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'fit 2'!$C$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>a</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'fit 2'!$B$5:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>116</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>232</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>464</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>696</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>928</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'fit 2'!$E$25:$E$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.5433019783579935</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.4918040551445935</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.4014353519810159</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.2367890716512302</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0914861007278438</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.96325390916619147</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="371746032"/>
-        <c:axId val="371746592"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="371746032"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ja-JP"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="371746592"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="371746592"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ja-JP"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="371746032"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4381,7 +4674,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4415,24 +4707,212 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:idx val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'fit3'!$C$4</c:f>
+              <c:f>'fit 2'!$D$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>a</c:v>
+                  <c:v>b</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'fit 2'!$B$5:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>464</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>696</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>928</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'fit 2'!$E$25:$E$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.5433019783579935</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4918040551445935</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4014353519810159</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2367890716512302</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0914861007278438</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.96325390916619147</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="426688656"/>
+        <c:axId val="426689216"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'fit 2'!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>b</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'fit 2'!$B$5:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>464</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>696</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>928</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'fit 2'!$D$25:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'fit 2'!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>a</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -4455,7 +4935,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'fit3'!$B$5:$B$10</c:f>
+              <c:f>'fit 2'!$B$5:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -4482,119 +4962,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'fit3'!$C$5:$C$10</c:f>
+              <c:f>'fit 2'!$E$25:$E$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.38350000000000001</c:v>
+                  <c:v>1.5433019783579935</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.36249999999999999</c:v>
+                  <c:v>1.4918040551445935</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.31840000000000002</c:v>
+                  <c:v>1.4014353519810159</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.29459999999999997</c:v>
+                  <c:v>1.2367890716512302</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.28010000000000002</c:v>
+                  <c:v>1.0914861007278438</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.30430000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'fit3'!$D$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>b</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'fit3'!$B$5:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>116</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>232</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>464</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>696</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>928</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'fit3'!$D$5:$D$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.37640000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.47320000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.66520000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.81499999999999995</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.93279999999999996</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.89</c:v>
+                  <c:v>0.96325390916619147</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4609,11 +4997,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="371749952"/>
-        <c:axId val="371750512"/>
+        <c:axId val="426688656"/>
+        <c:axId val="426689216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="371749952"/>
+        <c:axId val="426688656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4670,12 +5058,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371750512"/>
+        <c:crossAx val="426689216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="371750512"/>
+        <c:axId val="426689216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4732,7 +5120,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371749952"/>
+        <c:crossAx val="426688656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4746,7 +5134,451 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
       <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'fit3'!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>a</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'fit3'!$B$5:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>464</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>696</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>928</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'fit3'!$C$5:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.38350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.36249999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.31840000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.29459999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.28010000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.30430000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'fit3'!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>b</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'fit3'!$B$5:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>464</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>696</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>928</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'fit3'!$D$5:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.37640000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.47320000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.66520000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.81499999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.93279999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.89</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="426829568"/>
+        <c:axId val="426830128"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="426829568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="426830128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="426830128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="426829568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4813,7 +5645,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4828,7 +5660,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5056,11 +5887,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="371753872"/>
-        <c:axId val="371754432"/>
+        <c:axId val="389576480"/>
+        <c:axId val="389577040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="371753872"/>
+        <c:axId val="389576480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5117,12 +5948,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371754432"/>
+        <c:crossAx val="389577040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="371754432"/>
+        <c:axId val="389577040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5179,7 +6010,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371753872"/>
+        <c:crossAx val="389576480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5193,7 +6024,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5260,7 +6090,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5275,7 +6105,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5491,11 +6320,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="249034160"/>
-        <c:axId val="249029120"/>
+        <c:axId val="403639776"/>
+        <c:axId val="403640336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="249034160"/>
+        <c:axId val="403639776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5552,12 +6381,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="249029120"/>
+        <c:crossAx val="403640336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="249029120"/>
+        <c:axId val="403640336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5614,7 +6443,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="249034160"/>
+        <c:crossAx val="403639776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5628,7 +6457,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6015,6 +6843,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -9615,6 +10483,522 @@
 </file>
 
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -10203,6 +11587,43 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -10236,7 +11657,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10305,7 +11726,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10374,7 +11795,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10676,7 +12097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A18:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
@@ -11533,6 +12954,742 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D86"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="13.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="9.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4">
+        <v>1.1782426886005244E-9</v>
+      </c>
+      <c r="B2" s="5">
+        <v>-0.99838277802482045</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4">
+        <v>0.83001552430559766</v>
+      </c>
+      <c r="B3" s="5">
+        <v>-0.61322306275872585</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="4">
+        <v>1.7589948652665472</v>
+      </c>
+      <c r="B4" s="5">
+        <v>-0.41727233784336892</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4">
+        <v>2.7416603735437604</v>
+      </c>
+      <c r="B5" s="5">
+        <v>-0.32374989669132503</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="4">
+        <v>3.7576796987193877</v>
+      </c>
+      <c r="B6" s="5">
+        <v>-0.24633235668020714</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="4">
+        <v>4.7930546241118881</v>
+      </c>
+      <c r="B7" s="5">
+        <v>-0.19388056967841982</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="4">
+        <v>5.8349244772073154</v>
+      </c>
+      <c r="B8" s="5">
+        <v>-0.15963684492845132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="4">
+        <v>6.914758087843035</v>
+      </c>
+      <c r="B9" s="5">
+        <v>-0.13341414332915869</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="4">
+        <v>7.9833701226127234</v>
+      </c>
+      <c r="B10" s="5">
+        <v>-0.11190766491172366</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="4">
+        <v>9.0780800075120371</v>
+      </c>
+      <c r="B11" s="5">
+        <v>-0.10276467581223292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="4">
+        <v>10.15510136159808</v>
+      </c>
+      <c r="B12" s="5">
+        <v>-9.6729723684952029E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="4">
+        <v>11.251465412258712</v>
+      </c>
+      <c r="B13" s="5">
+        <v>-9.5309040439308212E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="4">
+        <v>12.439201033993605</v>
+      </c>
+      <c r="B14" s="5">
+        <v>-0.10109273789013917</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="4">
+        <v>7.8712636408795333E-8</v>
+      </c>
+      <c r="B15" s="5">
+        <v>-0.88456311129873444</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="4">
+        <v>0.60385484924843991</v>
+      </c>
+      <c r="B16" s="5">
+        <v>-0.73431037601183302</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="4">
+        <v>1.5489256315891522</v>
+      </c>
+      <c r="B17" s="5">
+        <v>-0.45582422382012289</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="4">
+        <v>2.5823189195798366</v>
+      </c>
+      <c r="B18" s="5">
+        <v>-0.31559189530742793</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="5">
+        <v>3.616329679161276</v>
+      </c>
+      <c r="B19" s="5">
+        <v>-0.23638655876496029</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="5">
+        <v>4.708119553395461</v>
+      </c>
+      <c r="B20" s="5">
+        <v>-0.18286450000625365</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="5">
+        <v>5.8224228299217398</v>
+      </c>
+      <c r="B21" s="5">
+        <v>-0.13944309096909246</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="5">
+        <v>6.9544037559349565</v>
+      </c>
+      <c r="B22" s="5">
+        <v>-0.11365219534445625</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="5">
+        <v>8.087888554101534</v>
+      </c>
+      <c r="B23" s="5">
+        <v>-9.6291770225417128E-2</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="5">
+        <v>9.2382312100566431</v>
+      </c>
+      <c r="B24" s="5">
+        <v>-8.7196058035180712E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="5">
+        <v>10.393042696659142</v>
+      </c>
+      <c r="B25" s="5">
+        <v>-7.3336627598270976E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="5">
+        <v>11.595556534490276</v>
+      </c>
+      <c r="B26" s="5">
+        <v>-7.2686623801271555E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="5">
+        <v>12.760909153627127</v>
+      </c>
+      <c r="B27" s="5">
+        <v>-7.4157477540880867E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="5">
+        <v>9.588996263687477E-10</v>
+      </c>
+      <c r="B28" s="5">
+        <v>-0.92434352155457233</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="5">
+        <v>0.86439544855037098</v>
+      </c>
+      <c r="B29" s="5">
+        <v>-0.59815475352698999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="5">
+        <v>1.8270880839220307</v>
+      </c>
+      <c r="B30" s="5">
+        <v>-0.40110825976505105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="5">
+        <v>2.8131835652496848</v>
+      </c>
+      <c r="B31" s="5">
+        <v>-0.29905086934963232</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="5">
+        <v>3.8888826306841788</v>
+      </c>
+      <c r="B32" s="5">
+        <v>-0.22886711701219875</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="5">
+        <v>4.9384663104565565</v>
+      </c>
+      <c r="B33" s="5">
+        <v>-0.1807216286625184</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="5">
+        <v>6.0396844916037837</v>
+      </c>
+      <c r="B34" s="5">
+        <v>-0.14746945952397716</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="5">
+        <v>7.1192576157988006</v>
+      </c>
+      <c r="B35" s="5">
+        <v>-0.12446302052617675</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="5">
+        <v>8.2334755863341869</v>
+      </c>
+      <c r="B36" s="5">
+        <v>-0.10663731850704128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="5">
+        <v>9.3529214808213137</v>
+      </c>
+      <c r="B37" s="5">
+        <v>-9.8306426218596199E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="5">
+        <v>10.457959603650322</v>
+      </c>
+      <c r="B38" s="5">
+        <v>-9.9555822995210042E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="5">
+        <v>7.7290840394539373E-9</v>
+      </c>
+      <c r="B39" s="5">
+        <v>-1.0562220670498046</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="5">
+        <v>0.78881789650508294</v>
+      </c>
+      <c r="B40" s="5">
+        <v>-0.63829438716569076</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="5">
+        <v>1.6964328109948899</v>
+      </c>
+      <c r="B41" s="5">
+        <v>-0.44991380847956175</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="5">
+        <v>2.6687025817170649</v>
+      </c>
+      <c r="B42" s="5">
+        <v>-0.34624293348388746</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="5">
+        <v>3.5894703995944859</v>
+      </c>
+      <c r="B43" s="5">
+        <v>-0.2628987505077478</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="5">
+        <v>4.5971902850329718</v>
+      </c>
+      <c r="B44" s="5">
+        <v>-0.20456733607634736</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="5">
+        <v>5.5707389170981036</v>
+      </c>
+      <c r="B45" s="5">
+        <v>-0.16376198830805255</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="5">
+        <v>6.6047566541380522</v>
+      </c>
+      <c r="B46" s="5">
+        <v>-0.13465652468058642</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="5">
+        <v>7.6222196992331996</v>
+      </c>
+      <c r="B47" s="5">
+        <v>-0.11284757798230438</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="5">
+        <v>8.6452885353400131</v>
+      </c>
+      <c r="B48" s="5">
+        <v>-0.10143163209276063</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="5">
+        <v>9.6871456706652967</v>
+      </c>
+      <c r="B49" s="5">
+        <v>-9.3923477877279726E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="5">
+        <v>10.740525300466734</v>
+      </c>
+      <c r="B50" s="5">
+        <v>-8.8678819210161741E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="5">
+        <v>11.799224683651081</v>
+      </c>
+      <c r="B51" s="5">
+        <v>-8.8437284218419121E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="5">
+        <v>12.842394085569522</v>
+      </c>
+      <c r="B52" s="5">
+        <v>-9.1079591729153364E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="5">
+        <v>13.939128383436827</v>
+      </c>
+      <c r="B53" s="5">
+        <v>-9.7868975529099345E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="5">
+        <v>2.531280308865322E-6</v>
+      </c>
+      <c r="B54" s="5">
+        <v>-1.0847555143299736</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="5">
+        <v>0.79227428895571161</v>
+      </c>
+      <c r="B55" s="5">
+        <v>-0.65187030070274132</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="5">
+        <v>1.6467493256652945</v>
+      </c>
+      <c r="B56" s="5">
+        <v>-0.4663050017803767</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="5">
+        <v>2.5786011719554747</v>
+      </c>
+      <c r="B57" s="5">
+        <v>-0.35793676363642857</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="5">
+        <v>3.4797714886515165</v>
+      </c>
+      <c r="B58" s="5">
+        <v>-0.27094612035282473</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="5">
+        <v>4.46032940890486</v>
+      </c>
+      <c r="B59" s="5">
+        <v>-0.20887469804261061</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="5">
+        <v>5.3807128307200633</v>
+      </c>
+      <c r="B60" s="5">
+        <v>-0.16786683170051719</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="5">
+        <v>6.3933386030602106</v>
+      </c>
+      <c r="B61" s="5">
+        <v>-0.13465370863326354</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="5">
+        <v>7.3773424148796956</v>
+      </c>
+      <c r="B62" s="5">
+        <v>-0.11345849214686354</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="5">
+        <v>8.3693944476711231</v>
+      </c>
+      <c r="B63" s="5">
+        <v>-0.10010041669404979</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="5">
+        <v>9.3997601185372393</v>
+      </c>
+      <c r="B64" s="5">
+        <v>-8.9122978407390807E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="5">
+        <v>10.42127381778735</v>
+      </c>
+      <c r="B65" s="5">
+        <v>-8.379704998582671E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="5">
+        <v>11.4366759110223</v>
+      </c>
+      <c r="B66" s="5">
+        <v>-8.4116996567273006E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="5">
+        <v>12.453888443639299</v>
+      </c>
+      <c r="B67" s="5">
+        <v>-8.3057565743880346E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="5">
+        <v>13.494096944178469</v>
+      </c>
+      <c r="B68" s="5">
+        <v>-8.323701551483409E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="5">
+        <v>14.54301115556521</v>
+      </c>
+      <c r="B69" s="5">
+        <v>-8.6810945894206348E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="5">
+        <v>7.9876845878364592E-11</v>
+      </c>
+      <c r="B70" s="5">
+        <v>-1.0995759540501888</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="5">
+        <v>0.78844564873822742</v>
+      </c>
+      <c r="B71" s="5">
+        <v>-0.66382382103749893</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="5">
+        <v>1.6206165472530574</v>
+      </c>
+      <c r="B72" s="5">
+        <v>-0.47891719273122968</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="5">
+        <v>2.5471234733867654</v>
+      </c>
+      <c r="B73" s="5">
+        <v>-0.3654935415169227</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="5">
+        <v>3.4239152124484211</v>
+      </c>
+      <c r="B74" s="5">
+        <v>-0.27541389757369683</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="5">
+        <v>4.3781385242079391</v>
+      </c>
+      <c r="B75" s="5">
+        <v>-0.21394633105404237</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="5">
+        <v>5.2990118274572842</v>
+      </c>
+      <c r="B76" s="5">
+        <v>-0.17055529153211646</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="5">
+        <v>6.2776536759509556</v>
+      </c>
+      <c r="B77" s="5">
+        <v>-0.13657785299767022</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="5">
+        <v>7.2305419317242237</v>
+      </c>
+      <c r="B78" s="5">
+        <v>-0.11350037110808553</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="5">
+        <v>8.203357726998961</v>
+      </c>
+      <c r="B79" s="5">
+        <v>-9.7663731690701416E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="5">
+        <v>9.2076430177192403</v>
+      </c>
+      <c r="B80" s="5">
+        <v>-8.9153432811833966E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="5">
+        <v>10.190712166579036</v>
+      </c>
+      <c r="B81" s="5">
+        <v>-8.2507518707066962E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="5">
+        <v>11.186873665065443</v>
+      </c>
+      <c r="B82" s="5">
+        <v>-7.688281361434246E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="5">
+        <v>12.189923798057709</v>
+      </c>
+      <c r="B83" s="5">
+        <v>-7.7829370367991313E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="5">
+        <v>13.186169417201416</v>
+      </c>
+      <c r="B84" s="5">
+        <v>-7.8348070535637859E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="5">
+        <v>14.215500696200856</v>
+      </c>
+      <c r="B85" s="5">
+        <v>-8.1000224638744456E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="5">
+        <v>15.2256821864807</v>
+      </c>
+      <c r="B86" s="5">
+        <v>-8.4421040578937179E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L19"/>
   <sheetViews>
@@ -11940,7 +14097,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q44"/>
   <sheetViews>
@@ -12579,7 +14736,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O49"/>
   <sheetViews>
@@ -13560,7 +15717,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L40"/>
   <sheetViews>

</xml_diff>